<commit_message>
Parse template cells as JSON
</commit_message>
<xml_diff>
--- a/src/assets/template.xlsx
+++ b/src/assets/template.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Guczi\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Programming\scheduler\src\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{034FF352-6B73-462C-9C04-261458200613}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CE8D8F6-FE13-4992-A00D-286BCDB91FDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="5" r:id="rId1"/>
+    <sheet name="Main" sheetId="5" r:id="rId1"/>
     <sheet name="Munka3" sheetId="3" state="hidden" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="77">
   <si>
     <t>órasz</t>
   </si>
@@ -181,9 +181,6 @@
     <t>${nextEmployee}</t>
   </si>
   <si>
-    <t xml:space="preserve"> 2018. Július - Beosztás</t>
-  </si>
-  <si>
     <t xml:space="preserve">2 havi munkaidő keret: 2018. 07. 01. - 2018. 08. 31.  július: 22X8=176 óra, augusztus:  22X8=176 óra        Összesen: 352 óra      SZ:  4 P: 5  FÜ: </t>
   </si>
   <si>
@@ -232,9 +229,6 @@
     </r>
   </si>
   <si>
-    <t>Mórahalom 2018. 06.15.</t>
-  </si>
-  <si>
     <t>készítette:</t>
   </si>
   <si>
@@ -262,25 +256,34 @@
     <t>${shiftEnd}</t>
   </si>
   <si>
-    <t>${startsAt(19)}</t>
+    <t>${startDate}</t>
   </si>
   <si>
-    <t>${startsAt(11)}</t>
+    <t xml:space="preserve"> ${year}. ${month} - Beosztás</t>
   </si>
   <si>
-    <t>${startsAt(9)}</t>
+    <t>${startsAt: [5]}</t>
   </si>
   <si>
-    <t>${startsAt(7)}</t>
+    <t>${shiftStart: []}</t>
   </si>
   <si>
-    <t>${startsAt(5)}</t>
+    <t>Mórahalom ${todayDate}</t>
   </si>
   <si>
-    <t>${presentBetween(17,18)}</t>
+    <t>${startsAt: [7]}</t>
   </si>
   <si>
-    <t>${startDate}</t>
+    <t>${startsAt: [9]}</t>
+  </si>
+  <si>
+    <t>${startsAt: [11]}</t>
+  </si>
+  <si>
+    <t>${startsAt: [19]}</t>
+  </si>
+  <si>
+    <t>${presentBetween: [17,18]}</t>
   </si>
 </sst>
 </file>
@@ -290,7 +293,7 @@
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="mmm\ d/"/>
     <numFmt numFmtId="165" formatCode="m\.\ d\.;@"/>
-    <numFmt numFmtId="168" formatCode="d"/>
+    <numFmt numFmtId="166" formatCode="d"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -1054,7 +1057,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="126">
+  <cellXfs count="121">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1090,9 +1093,6 @@
       <alignment vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection locked="0"/>
@@ -1116,9 +1116,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="1" fontId="5" fillId="3" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -1126,9 +1123,6 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="3" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1142,9 +1136,6 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1177,15 +1168,6 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -1200,12 +1182,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
@@ -1244,78 +1220,20 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="1" fontId="6" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" fillId="3" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="166" fontId="9" fillId="4" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" fillId="3" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="6" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="6" fillId="3" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="6" fillId="3" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" fillId="3" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="3" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="3" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="3" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="5" fillId="3" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1324,31 +1242,23 @@
     <xf numFmtId="1" fontId="5" fillId="3" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="1" fontId="6" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" fillId="3" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1418,38 +1328,108 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="9" fillId="4" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="3" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="3" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="3" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="3" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="3" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="3" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="3" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="3" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="3" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="3" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="9" fillId="4" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
@@ -1883,8 +1863,8 @@
   </sheetPr>
   <dimension ref="A1:AO36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="Y13" sqref="Y13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2471,1677 +2451,2160 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:41" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="99" t="s">
-        <v>49</v>
-      </c>
-      <c r="B1" s="99"/>
-      <c r="C1" s="99"/>
-      <c r="D1" s="99"/>
-      <c r="E1" s="99"/>
-      <c r="F1" s="99"/>
-      <c r="G1" s="99"/>
-      <c r="H1" s="99"/>
-      <c r="I1" s="99"/>
-      <c r="J1" s="99"/>
-      <c r="K1" s="99"/>
-      <c r="L1" s="99"/>
-      <c r="M1" s="99"/>
-      <c r="N1" s="99"/>
-      <c r="O1" s="99"/>
-      <c r="P1" s="99"/>
-      <c r="Q1" s="99"/>
-      <c r="R1" s="99"/>
-      <c r="S1" s="99"/>
-      <c r="T1" s="99"/>
-      <c r="U1" s="99"/>
-      <c r="V1" s="99"/>
-      <c r="W1" s="99"/>
-      <c r="X1" s="99"/>
-      <c r="Y1" s="99"/>
-      <c r="Z1" s="99"/>
-      <c r="AA1" s="99"/>
-      <c r="AB1" s="99"/>
-      <c r="AC1" s="99"/>
-      <c r="AD1" s="99"/>
-      <c r="AE1" s="99"/>
-      <c r="AF1" s="99"/>
-      <c r="AG1" s="99"/>
-      <c r="AH1" s="99"/>
-      <c r="AI1" s="99"/>
-      <c r="AJ1" s="99"/>
-      <c r="AK1" s="99"/>
-      <c r="AL1" s="99"/>
-      <c r="AM1" s="99"/>
-      <c r="AN1" s="99"/>
-      <c r="AO1" s="99"/>
+      <c r="A1" s="69" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" s="69"/>
+      <c r="C1" s="69"/>
+      <c r="D1" s="69"/>
+      <c r="E1" s="69"/>
+      <c r="F1" s="69"/>
+      <c r="G1" s="69"/>
+      <c r="H1" s="69"/>
+      <c r="I1" s="69"/>
+      <c r="J1" s="69"/>
+      <c r="K1" s="69"/>
+      <c r="L1" s="69"/>
+      <c r="M1" s="69"/>
+      <c r="N1" s="69"/>
+      <c r="O1" s="69"/>
+      <c r="P1" s="69"/>
+      <c r="Q1" s="69"/>
+      <c r="R1" s="69"/>
+      <c r="S1" s="69"/>
+      <c r="T1" s="69"/>
+      <c r="U1" s="69"/>
+      <c r="V1" s="69"/>
+      <c r="W1" s="69"/>
+      <c r="X1" s="69"/>
+      <c r="Y1" s="69"/>
+      <c r="Z1" s="69"/>
+      <c r="AA1" s="69"/>
+      <c r="AB1" s="69"/>
+      <c r="AC1" s="69"/>
+      <c r="AD1" s="69"/>
+      <c r="AE1" s="69"/>
+      <c r="AF1" s="69"/>
+      <c r="AG1" s="69"/>
+      <c r="AH1" s="69"/>
+      <c r="AI1" s="69"/>
+      <c r="AJ1" s="69"/>
+      <c r="AK1" s="69"/>
+      <c r="AL1" s="69"/>
+      <c r="AM1" s="69"/>
+      <c r="AN1" s="69"/>
+      <c r="AO1" s="69"/>
     </row>
     <row r="2" spans="1:41" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="99" t="s">
+      <c r="A2" s="69" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="99"/>
-      <c r="C2" s="99"/>
-      <c r="D2" s="99"/>
-      <c r="E2" s="99"/>
-      <c r="F2" s="99"/>
-      <c r="G2" s="99"/>
-      <c r="H2" s="99"/>
-      <c r="I2" s="99"/>
-      <c r="J2" s="99"/>
-      <c r="K2" s="99"/>
-      <c r="L2" s="99"/>
-      <c r="M2" s="99"/>
-      <c r="N2" s="99"/>
-      <c r="O2" s="99"/>
-      <c r="P2" s="99"/>
-      <c r="Q2" s="99"/>
-      <c r="R2" s="99"/>
-      <c r="S2" s="99"/>
-      <c r="T2" s="99"/>
-      <c r="U2" s="99"/>
-      <c r="V2" s="99"/>
-      <c r="W2" s="99"/>
-      <c r="X2" s="99"/>
-      <c r="Y2" s="99"/>
-      <c r="Z2" s="99"/>
-      <c r="AA2" s="99"/>
-      <c r="AB2" s="99"/>
-      <c r="AC2" s="99"/>
-      <c r="AD2" s="99"/>
-      <c r="AE2" s="99"/>
-      <c r="AF2" s="99"/>
-      <c r="AG2" s="99"/>
-      <c r="AH2" s="99"/>
-      <c r="AI2" s="99"/>
-      <c r="AJ2" s="99"/>
-      <c r="AK2" s="99"/>
-      <c r="AL2" s="99"/>
-      <c r="AM2" s="99"/>
-      <c r="AN2" s="99"/>
-      <c r="AO2" s="99"/>
+      <c r="B2" s="69"/>
+      <c r="C2" s="69"/>
+      <c r="D2" s="69"/>
+      <c r="E2" s="69"/>
+      <c r="F2" s="69"/>
+      <c r="G2" s="69"/>
+      <c r="H2" s="69"/>
+      <c r="I2" s="69"/>
+      <c r="J2" s="69"/>
+      <c r="K2" s="69"/>
+      <c r="L2" s="69"/>
+      <c r="M2" s="69"/>
+      <c r="N2" s="69"/>
+      <c r="O2" s="69"/>
+      <c r="P2" s="69"/>
+      <c r="Q2" s="69"/>
+      <c r="R2" s="69"/>
+      <c r="S2" s="69"/>
+      <c r="T2" s="69"/>
+      <c r="U2" s="69"/>
+      <c r="V2" s="69"/>
+      <c r="W2" s="69"/>
+      <c r="X2" s="69"/>
+      <c r="Y2" s="69"/>
+      <c r="Z2" s="69"/>
+      <c r="AA2" s="69"/>
+      <c r="AB2" s="69"/>
+      <c r="AC2" s="69"/>
+      <c r="AD2" s="69"/>
+      <c r="AE2" s="69"/>
+      <c r="AF2" s="69"/>
+      <c r="AG2" s="69"/>
+      <c r="AH2" s="69"/>
+      <c r="AI2" s="69"/>
+      <c r="AJ2" s="69"/>
+      <c r="AK2" s="69"/>
+      <c r="AL2" s="69"/>
+      <c r="AM2" s="69"/>
+      <c r="AN2" s="69"/>
+      <c r="AO2" s="69"/>
     </row>
     <row r="3" spans="1:41" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="100" t="s">
-        <v>50</v>
-      </c>
-      <c r="B3" s="100"/>
-      <c r="C3" s="100"/>
-      <c r="D3" s="100"/>
-      <c r="E3" s="100"/>
-      <c r="F3" s="100"/>
-      <c r="G3" s="100"/>
-      <c r="H3" s="100"/>
-      <c r="I3" s="100"/>
-      <c r="J3" s="100"/>
-      <c r="K3" s="100"/>
-      <c r="L3" s="100"/>
-      <c r="M3" s="100"/>
-      <c r="N3" s="100"/>
-      <c r="O3" s="100"/>
-      <c r="P3" s="100"/>
-      <c r="Q3" s="100"/>
-      <c r="R3" s="100"/>
-      <c r="S3" s="100"/>
-      <c r="T3" s="100"/>
-      <c r="U3" s="100"/>
-      <c r="V3" s="100"/>
-      <c r="W3" s="100"/>
-      <c r="X3" s="100"/>
-      <c r="Y3" s="100"/>
-      <c r="Z3" s="100"/>
-      <c r="AA3" s="100"/>
-      <c r="AB3" s="100"/>
-      <c r="AC3" s="100"/>
-      <c r="AD3" s="100"/>
-      <c r="AE3" s="100"/>
-      <c r="AF3" s="100"/>
-      <c r="AG3" s="100"/>
-      <c r="AH3" s="100"/>
-      <c r="AI3" s="100"/>
-      <c r="AJ3" s="100"/>
-      <c r="AK3" s="100"/>
-      <c r="AL3" s="100"/>
-      <c r="AM3" s="100"/>
-      <c r="AN3" s="100"/>
-      <c r="AO3" s="100"/>
+      <c r="A3" s="70" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" s="70"/>
+      <c r="C3" s="70"/>
+      <c r="D3" s="70"/>
+      <c r="E3" s="70"/>
+      <c r="F3" s="70"/>
+      <c r="G3" s="70"/>
+      <c r="H3" s="70"/>
+      <c r="I3" s="70"/>
+      <c r="J3" s="70"/>
+      <c r="K3" s="70"/>
+      <c r="L3" s="70"/>
+      <c r="M3" s="70"/>
+      <c r="N3" s="70"/>
+      <c r="O3" s="70"/>
+      <c r="P3" s="70"/>
+      <c r="Q3" s="70"/>
+      <c r="R3" s="70"/>
+      <c r="S3" s="70"/>
+      <c r="T3" s="70"/>
+      <c r="U3" s="70"/>
+      <c r="V3" s="70"/>
+      <c r="W3" s="70"/>
+      <c r="X3" s="70"/>
+      <c r="Y3" s="70"/>
+      <c r="Z3" s="70"/>
+      <c r="AA3" s="70"/>
+      <c r="AB3" s="70"/>
+      <c r="AC3" s="70"/>
+      <c r="AD3" s="70"/>
+      <c r="AE3" s="70"/>
+      <c r="AF3" s="70"/>
+      <c r="AG3" s="70"/>
+      <c r="AH3" s="70"/>
+      <c r="AI3" s="70"/>
+      <c r="AJ3" s="70"/>
+      <c r="AK3" s="70"/>
+      <c r="AL3" s="70"/>
+      <c r="AM3" s="70"/>
+      <c r="AN3" s="70"/>
+      <c r="AO3" s="70"/>
     </row>
-    <row r="4" spans="1:41" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="40" t="s">
+    <row r="4" spans="1:41" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="41" t="s">
-        <v>73</v>
-      </c>
-      <c r="C4" s="41"/>
-      <c r="D4" s="41"/>
-      <c r="E4" s="41"/>
-      <c r="F4" s="41"/>
-      <c r="G4" s="41"/>
-      <c r="H4" s="41"/>
-      <c r="I4" s="41"/>
-      <c r="J4" s="41"/>
-      <c r="K4" s="41"/>
-      <c r="L4" s="41"/>
-      <c r="M4" s="41"/>
-      <c r="N4" s="41"/>
-      <c r="O4" s="41"/>
-      <c r="P4" s="41"/>
-      <c r="Q4" s="41"/>
-      <c r="R4" s="41"/>
-      <c r="S4" s="41"/>
-      <c r="T4" s="41"/>
-      <c r="U4" s="41"/>
-      <c r="V4" s="41"/>
-      <c r="W4" s="41"/>
-      <c r="X4" s="41"/>
-      <c r="Y4" s="41"/>
-      <c r="Z4" s="41"/>
-      <c r="AA4" s="41"/>
-      <c r="AB4" s="41"/>
-      <c r="AC4" s="41"/>
-      <c r="AD4" s="41"/>
-      <c r="AE4" s="41"/>
-      <c r="AF4" s="41"/>
-      <c r="AG4" s="101"/>
-      <c r="AH4" s="104" t="s">
+      <c r="B4" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="C4" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="D4" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="E4" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="F4" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="G4" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="H4" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="I4" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="J4" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="K4" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="L4" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="M4" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="N4" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="O4" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="P4" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q4" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="R4" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="S4" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="T4" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="U4" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="V4" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="W4" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="X4" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="Y4" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="Z4" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA4" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="AB4" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="AC4" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="AD4" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="AE4" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="AF4" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="AG4" s="71"/>
+      <c r="AH4" s="74" t="s">
         <v>28</v>
       </c>
-      <c r="AI4" s="105"/>
-      <c r="AJ4" s="105"/>
-      <c r="AK4" s="105"/>
-      <c r="AL4" s="106"/>
-      <c r="AM4" s="42" t="e">
-        <f>AH12+AH16+#REF!+#REF!+#REF!+#REF!+#REF!+#REF!+#REF!+#REF!+#REF!+#REF!+#REF!+#REF!+#REF!+#REF!+#REF!+#REF!+#REF!+#REF!+#REF!+#REF!+#REF!+#REF!+#REF!+#REF!+#REF!+#REF!+#REF!+#REF!</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AN4" s="43"/>
-      <c r="AO4" s="107" t="s">
+      <c r="AI4" s="75"/>
+      <c r="AJ4" s="75"/>
+      <c r="AK4" s="75"/>
+      <c r="AL4" s="76"/>
+      <c r="AM4" s="38"/>
+      <c r="AN4" s="39"/>
+      <c r="AO4" s="77" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:41" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="44" t="s">
+      <c r="A5" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="45" t="s">
+      <c r="B5" s="37" t="s">
         <v>72</v>
       </c>
-      <c r="C5" s="45"/>
-      <c r="D5" s="45"/>
-      <c r="E5" s="45"/>
-      <c r="F5" s="45"/>
-      <c r="G5" s="45"/>
-      <c r="H5" s="45"/>
-      <c r="I5" s="45"/>
-      <c r="J5" s="45"/>
-      <c r="K5" s="45"/>
-      <c r="L5" s="45"/>
-      <c r="M5" s="45"/>
-      <c r="N5" s="45"/>
-      <c r="O5" s="45"/>
-      <c r="P5" s="45"/>
-      <c r="Q5" s="45"/>
-      <c r="R5" s="45"/>
-      <c r="S5" s="45"/>
-      <c r="T5" s="45"/>
-      <c r="U5" s="45"/>
-      <c r="V5" s="45"/>
-      <c r="W5" s="45"/>
-      <c r="X5" s="45"/>
-      <c r="Y5" s="45"/>
-      <c r="Z5" s="45"/>
-      <c r="AA5" s="45"/>
-      <c r="AB5" s="45"/>
-      <c r="AC5" s="45"/>
-      <c r="AD5" s="45"/>
-      <c r="AE5" s="45"/>
-      <c r="AF5" s="45"/>
-      <c r="AG5" s="102"/>
-      <c r="AH5" s="109"/>
-      <c r="AI5" s="110"/>
-      <c r="AJ5" s="110"/>
-      <c r="AK5" s="110"/>
-      <c r="AL5" s="110"/>
-      <c r="AM5" s="110"/>
-      <c r="AN5" s="111"/>
-      <c r="AO5" s="108"/>
+      <c r="C5" s="37" t="s">
+        <v>72</v>
+      </c>
+      <c r="D5" s="37" t="s">
+        <v>72</v>
+      </c>
+      <c r="E5" s="37" t="s">
+        <v>72</v>
+      </c>
+      <c r="F5" s="37" t="s">
+        <v>72</v>
+      </c>
+      <c r="G5" s="37" t="s">
+        <v>72</v>
+      </c>
+      <c r="H5" s="37" t="s">
+        <v>72</v>
+      </c>
+      <c r="I5" s="37" t="s">
+        <v>72</v>
+      </c>
+      <c r="J5" s="37" t="s">
+        <v>72</v>
+      </c>
+      <c r="K5" s="37" t="s">
+        <v>72</v>
+      </c>
+      <c r="L5" s="37" t="s">
+        <v>72</v>
+      </c>
+      <c r="M5" s="37" t="s">
+        <v>72</v>
+      </c>
+      <c r="N5" s="37" t="s">
+        <v>72</v>
+      </c>
+      <c r="O5" s="37" t="s">
+        <v>72</v>
+      </c>
+      <c r="P5" s="37" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q5" s="37" t="s">
+        <v>72</v>
+      </c>
+      <c r="R5" s="37" t="s">
+        <v>72</v>
+      </c>
+      <c r="S5" s="37" t="s">
+        <v>72</v>
+      </c>
+      <c r="T5" s="37" t="s">
+        <v>72</v>
+      </c>
+      <c r="U5" s="37" t="s">
+        <v>72</v>
+      </c>
+      <c r="V5" s="37" t="s">
+        <v>72</v>
+      </c>
+      <c r="W5" s="37" t="s">
+        <v>72</v>
+      </c>
+      <c r="X5" s="37" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y5" s="37" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z5" s="37" t="s">
+        <v>72</v>
+      </c>
+      <c r="AA5" s="37" t="s">
+        <v>72</v>
+      </c>
+      <c r="AB5" s="37" t="s">
+        <v>72</v>
+      </c>
+      <c r="AC5" s="37" t="s">
+        <v>72</v>
+      </c>
+      <c r="AD5" s="37" t="s">
+        <v>72</v>
+      </c>
+      <c r="AE5" s="37" t="s">
+        <v>72</v>
+      </c>
+      <c r="AF5" s="37" t="s">
+        <v>72</v>
+      </c>
+      <c r="AG5" s="72"/>
+      <c r="AH5" s="79"/>
+      <c r="AI5" s="80"/>
+      <c r="AJ5" s="80"/>
+      <c r="AK5" s="80"/>
+      <c r="AL5" s="80"/>
+      <c r="AM5" s="80"/>
+      <c r="AN5" s="81"/>
+      <c r="AO5" s="78"/>
     </row>
     <row r="6" spans="1:41" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="44" t="s">
+      <c r="A6" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="B6" s="45" t="s">
-        <v>71</v>
-      </c>
-      <c r="C6" s="45"/>
-      <c r="D6" s="45"/>
-      <c r="E6" s="45"/>
-      <c r="F6" s="45"/>
-      <c r="G6" s="45"/>
-      <c r="H6" s="45"/>
-      <c r="I6" s="45"/>
-      <c r="J6" s="45"/>
-      <c r="K6" s="45"/>
-      <c r="L6" s="45"/>
-      <c r="M6" s="45"/>
-      <c r="N6" s="45"/>
-      <c r="O6" s="45"/>
-      <c r="P6" s="45"/>
-      <c r="Q6" s="45"/>
-      <c r="R6" s="45"/>
-      <c r="S6" s="45"/>
-      <c r="T6" s="45"/>
-      <c r="U6" s="45"/>
-      <c r="V6" s="45"/>
-      <c r="W6" s="45"/>
-      <c r="X6" s="45"/>
-      <c r="Y6" s="45"/>
-      <c r="Z6" s="45"/>
-      <c r="AA6" s="45"/>
-      <c r="AB6" s="45"/>
-      <c r="AC6" s="45"/>
-      <c r="AD6" s="45"/>
-      <c r="AE6" s="45"/>
-      <c r="AF6" s="45"/>
-      <c r="AG6" s="102"/>
-      <c r="AH6" s="46"/>
-      <c r="AI6" s="47"/>
-      <c r="AJ6" s="47"/>
-      <c r="AK6" s="47"/>
-      <c r="AL6" s="47"/>
-      <c r="AM6" s="47"/>
-      <c r="AN6" s="48"/>
-      <c r="AO6" s="49">
+      <c r="B6" s="37" t="s">
+        <v>73</v>
+      </c>
+      <c r="C6" s="37" t="s">
+        <v>73</v>
+      </c>
+      <c r="D6" s="37" t="s">
+        <v>73</v>
+      </c>
+      <c r="E6" s="37" t="s">
+        <v>73</v>
+      </c>
+      <c r="F6" s="37" t="s">
+        <v>73</v>
+      </c>
+      <c r="G6" s="37" t="s">
+        <v>73</v>
+      </c>
+      <c r="H6" s="37" t="s">
+        <v>73</v>
+      </c>
+      <c r="I6" s="37" t="s">
+        <v>73</v>
+      </c>
+      <c r="J6" s="37" t="s">
+        <v>73</v>
+      </c>
+      <c r="K6" s="37" t="s">
+        <v>73</v>
+      </c>
+      <c r="L6" s="37" t="s">
+        <v>73</v>
+      </c>
+      <c r="M6" s="37" t="s">
+        <v>73</v>
+      </c>
+      <c r="N6" s="37" t="s">
+        <v>73</v>
+      </c>
+      <c r="O6" s="37" t="s">
+        <v>73</v>
+      </c>
+      <c r="P6" s="37" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q6" s="37" t="s">
+        <v>73</v>
+      </c>
+      <c r="R6" s="37" t="s">
+        <v>73</v>
+      </c>
+      <c r="S6" s="37" t="s">
+        <v>73</v>
+      </c>
+      <c r="T6" s="37" t="s">
+        <v>73</v>
+      </c>
+      <c r="U6" s="37" t="s">
+        <v>73</v>
+      </c>
+      <c r="V6" s="37" t="s">
+        <v>73</v>
+      </c>
+      <c r="W6" s="37" t="s">
+        <v>73</v>
+      </c>
+      <c r="X6" s="37" t="s">
+        <v>73</v>
+      </c>
+      <c r="Y6" s="37" t="s">
+        <v>73</v>
+      </c>
+      <c r="Z6" s="37" t="s">
+        <v>73</v>
+      </c>
+      <c r="AA6" s="37" t="s">
+        <v>73</v>
+      </c>
+      <c r="AB6" s="37" t="s">
+        <v>73</v>
+      </c>
+      <c r="AC6" s="37" t="s">
+        <v>73</v>
+      </c>
+      <c r="AD6" s="37" t="s">
+        <v>73</v>
+      </c>
+      <c r="AE6" s="37" t="s">
+        <v>73</v>
+      </c>
+      <c r="AF6" s="37" t="s">
+        <v>73</v>
+      </c>
+      <c r="AG6" s="72"/>
+      <c r="AH6" s="59"/>
+      <c r="AI6" s="60"/>
+      <c r="AJ6" s="60"/>
+      <c r="AK6" s="60"/>
+      <c r="AL6" s="60"/>
+      <c r="AM6" s="60"/>
+      <c r="AN6" s="61"/>
+      <c r="AO6" s="42">
         <v>176</v>
       </c>
     </row>
     <row r="7" spans="1:41" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="44" t="s">
+      <c r="A7" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="45" t="s">
-        <v>70</v>
-      </c>
-      <c r="C7" s="45"/>
-      <c r="D7" s="45"/>
-      <c r="E7" s="45"/>
-      <c r="F7" s="45"/>
-      <c r="G7" s="45"/>
-      <c r="H7" s="45"/>
-      <c r="I7" s="45"/>
-      <c r="J7" s="45"/>
-      <c r="K7" s="45"/>
-      <c r="L7" s="45"/>
-      <c r="M7" s="45"/>
-      <c r="N7" s="45"/>
-      <c r="O7" s="45"/>
-      <c r="P7" s="45"/>
-      <c r="Q7" s="45"/>
-      <c r="R7" s="45"/>
-      <c r="S7" s="45"/>
-      <c r="T7" s="45"/>
-      <c r="U7" s="45"/>
-      <c r="V7" s="45"/>
-      <c r="W7" s="45"/>
-      <c r="X7" s="45"/>
-      <c r="Y7" s="45"/>
-      <c r="Z7" s="45"/>
-      <c r="AA7" s="45"/>
-      <c r="AB7" s="45"/>
-      <c r="AC7" s="45"/>
-      <c r="AD7" s="45"/>
-      <c r="AE7" s="45"/>
-      <c r="AF7" s="45"/>
-      <c r="AG7" s="102"/>
-      <c r="AH7" s="112" t="s">
+      <c r="B7" s="37" t="s">
+        <v>74</v>
+      </c>
+      <c r="C7" s="37" t="s">
+        <v>74</v>
+      </c>
+      <c r="D7" s="37" t="s">
+        <v>74</v>
+      </c>
+      <c r="E7" s="37" t="s">
+        <v>74</v>
+      </c>
+      <c r="F7" s="37" t="s">
+        <v>74</v>
+      </c>
+      <c r="G7" s="37" t="s">
+        <v>74</v>
+      </c>
+      <c r="H7" s="37" t="s">
+        <v>74</v>
+      </c>
+      <c r="I7" s="37" t="s">
+        <v>74</v>
+      </c>
+      <c r="J7" s="37" t="s">
+        <v>74</v>
+      </c>
+      <c r="K7" s="37" t="s">
+        <v>74</v>
+      </c>
+      <c r="L7" s="37" t="s">
+        <v>74</v>
+      </c>
+      <c r="M7" s="37" t="s">
+        <v>74</v>
+      </c>
+      <c r="N7" s="37" t="s">
+        <v>74</v>
+      </c>
+      <c r="O7" s="37" t="s">
+        <v>74</v>
+      </c>
+      <c r="P7" s="37" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q7" s="37" t="s">
+        <v>74</v>
+      </c>
+      <c r="R7" s="37" t="s">
+        <v>74</v>
+      </c>
+      <c r="S7" s="37" t="s">
+        <v>74</v>
+      </c>
+      <c r="T7" s="37" t="s">
+        <v>74</v>
+      </c>
+      <c r="U7" s="37" t="s">
+        <v>74</v>
+      </c>
+      <c r="V7" s="37" t="s">
+        <v>74</v>
+      </c>
+      <c r="W7" s="37" t="s">
+        <v>74</v>
+      </c>
+      <c r="X7" s="37" t="s">
+        <v>74</v>
+      </c>
+      <c r="Y7" s="37" t="s">
+        <v>74</v>
+      </c>
+      <c r="Z7" s="37" t="s">
+        <v>74</v>
+      </c>
+      <c r="AA7" s="37" t="s">
+        <v>74</v>
+      </c>
+      <c r="AB7" s="37" t="s">
+        <v>74</v>
+      </c>
+      <c r="AC7" s="37" t="s">
+        <v>74</v>
+      </c>
+      <c r="AD7" s="37" t="s">
+        <v>74</v>
+      </c>
+      <c r="AE7" s="37" t="s">
+        <v>74</v>
+      </c>
+      <c r="AF7" s="37" t="s">
+        <v>74</v>
+      </c>
+      <c r="AG7" s="72"/>
+      <c r="AH7" s="82" t="s">
         <v>29</v>
       </c>
-      <c r="AI7" s="113"/>
-      <c r="AJ7" s="113"/>
-      <c r="AK7" s="113"/>
-      <c r="AL7" s="114"/>
-      <c r="AM7" s="50" t="e">
-        <f>AI12+AI16+#REF!+#REF!+#REF!+#REF!+#REF!+#REF!+#REF!+#REF!+#REF!+#REF!+#REF!+#REF!+#REF!+#REF!+#REF!+#REF!+#REF!</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AN7" s="51"/>
-      <c r="AO7" s="52"/>
+      <c r="AI7" s="83"/>
+      <c r="AJ7" s="83"/>
+      <c r="AK7" s="83"/>
+      <c r="AL7" s="84"/>
+      <c r="AM7" s="43"/>
+      <c r="AN7" s="44"/>
+      <c r="AO7" s="45"/>
     </row>
-    <row r="8" spans="1:41" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="44" t="s">
+    <row r="8" spans="1:41" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="45" t="s">
-        <v>74</v>
-      </c>
-      <c r="C8" s="45"/>
-      <c r="D8" s="45"/>
-      <c r="E8" s="45"/>
-      <c r="F8" s="45"/>
-      <c r="G8" s="45"/>
-      <c r="H8" s="45"/>
-      <c r="I8" s="45"/>
-      <c r="J8" s="45"/>
-      <c r="K8" s="45"/>
-      <c r="L8" s="45"/>
-      <c r="M8" s="45"/>
-      <c r="N8" s="45"/>
-      <c r="O8" s="45"/>
-      <c r="P8" s="45"/>
-      <c r="Q8" s="45"/>
-      <c r="R8" s="45"/>
-      <c r="S8" s="45"/>
-      <c r="T8" s="45"/>
-      <c r="U8" s="45"/>
-      <c r="V8" s="45"/>
-      <c r="W8" s="45"/>
-      <c r="X8" s="45"/>
-      <c r="Y8" s="45"/>
-      <c r="Z8" s="45"/>
-      <c r="AA8" s="45"/>
-      <c r="AB8" s="45"/>
-      <c r="AC8" s="45"/>
-      <c r="AD8" s="45"/>
-      <c r="AE8" s="45"/>
-      <c r="AF8" s="45"/>
-      <c r="AG8" s="102"/>
-      <c r="AH8" s="115"/>
-      <c r="AI8" s="116"/>
-      <c r="AJ8" s="116"/>
-      <c r="AK8" s="116"/>
-      <c r="AL8" s="116"/>
-      <c r="AM8" s="116"/>
-      <c r="AN8" s="117"/>
-      <c r="AO8" s="52"/>
+      <c r="B8" s="41" t="s">
+        <v>76</v>
+      </c>
+      <c r="C8" s="41" t="s">
+        <v>76</v>
+      </c>
+      <c r="D8" s="41" t="s">
+        <v>76</v>
+      </c>
+      <c r="E8" s="41" t="s">
+        <v>76</v>
+      </c>
+      <c r="F8" s="41" t="s">
+        <v>76</v>
+      </c>
+      <c r="G8" s="41" t="s">
+        <v>76</v>
+      </c>
+      <c r="H8" s="41" t="s">
+        <v>76</v>
+      </c>
+      <c r="I8" s="41" t="s">
+        <v>76</v>
+      </c>
+      <c r="J8" s="41" t="s">
+        <v>76</v>
+      </c>
+      <c r="K8" s="41" t="s">
+        <v>76</v>
+      </c>
+      <c r="L8" s="41" t="s">
+        <v>76</v>
+      </c>
+      <c r="M8" s="41" t="s">
+        <v>76</v>
+      </c>
+      <c r="N8" s="41" t="s">
+        <v>76</v>
+      </c>
+      <c r="O8" s="41" t="s">
+        <v>76</v>
+      </c>
+      <c r="P8" s="41" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q8" s="41" t="s">
+        <v>76</v>
+      </c>
+      <c r="R8" s="41" t="s">
+        <v>76</v>
+      </c>
+      <c r="S8" s="41" t="s">
+        <v>76</v>
+      </c>
+      <c r="T8" s="41" t="s">
+        <v>76</v>
+      </c>
+      <c r="U8" s="41" t="s">
+        <v>76</v>
+      </c>
+      <c r="V8" s="41" t="s">
+        <v>76</v>
+      </c>
+      <c r="W8" s="41" t="s">
+        <v>76</v>
+      </c>
+      <c r="X8" s="41" t="s">
+        <v>76</v>
+      </c>
+      <c r="Y8" s="41" t="s">
+        <v>76</v>
+      </c>
+      <c r="Z8" s="41" t="s">
+        <v>76</v>
+      </c>
+      <c r="AA8" s="41" t="s">
+        <v>76</v>
+      </c>
+      <c r="AB8" s="41" t="s">
+        <v>76</v>
+      </c>
+      <c r="AC8" s="41" t="s">
+        <v>76</v>
+      </c>
+      <c r="AD8" s="41" t="s">
+        <v>76</v>
+      </c>
+      <c r="AE8" s="41" t="s">
+        <v>76</v>
+      </c>
+      <c r="AF8" s="41" t="s">
+        <v>76</v>
+      </c>
+      <c r="AG8" s="72"/>
+      <c r="AH8" s="85"/>
+      <c r="AI8" s="86"/>
+      <c r="AJ8" s="86"/>
+      <c r="AK8" s="86"/>
+      <c r="AL8" s="86"/>
+      <c r="AM8" s="86"/>
+      <c r="AN8" s="87"/>
+      <c r="AO8" s="45"/>
     </row>
     <row r="9" spans="1:41" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="53" t="s">
+      <c r="A9" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="54" t="s">
-        <v>69</v>
-      </c>
-      <c r="C9" s="54"/>
-      <c r="D9" s="54"/>
-      <c r="E9" s="54"/>
-      <c r="F9" s="54"/>
-      <c r="G9" s="54"/>
-      <c r="H9" s="54"/>
-      <c r="I9" s="54"/>
-      <c r="J9" s="54"/>
-      <c r="K9" s="54"/>
-      <c r="L9" s="54"/>
-      <c r="M9" s="54"/>
-      <c r="N9" s="54"/>
-      <c r="O9" s="54"/>
-      <c r="P9" s="54"/>
-      <c r="Q9" s="54"/>
-      <c r="R9" s="54"/>
-      <c r="S9" s="54"/>
-      <c r="T9" s="54"/>
-      <c r="U9" s="54"/>
-      <c r="V9" s="54"/>
-      <c r="W9" s="54"/>
-      <c r="X9" s="54"/>
-      <c r="Y9" s="54"/>
-      <c r="Z9" s="54"/>
-      <c r="AA9" s="54"/>
-      <c r="AB9" s="54"/>
-      <c r="AC9" s="54"/>
-      <c r="AD9" s="54"/>
-      <c r="AE9" s="54"/>
-      <c r="AF9" s="54"/>
-      <c r="AG9" s="103"/>
-      <c r="AH9" s="118"/>
-      <c r="AI9" s="119"/>
-      <c r="AJ9" s="119"/>
-      <c r="AK9" s="119"/>
-      <c r="AL9" s="119"/>
-      <c r="AM9" s="119"/>
-      <c r="AN9" s="120"/>
-      <c r="AO9" s="55"/>
+      <c r="B9" s="37" t="s">
+        <v>75</v>
+      </c>
+      <c r="C9" s="37" t="s">
+        <v>75</v>
+      </c>
+      <c r="D9" s="37" t="s">
+        <v>75</v>
+      </c>
+      <c r="E9" s="37" t="s">
+        <v>75</v>
+      </c>
+      <c r="F9" s="37" t="s">
+        <v>75</v>
+      </c>
+      <c r="G9" s="37" t="s">
+        <v>75</v>
+      </c>
+      <c r="H9" s="37" t="s">
+        <v>75</v>
+      </c>
+      <c r="I9" s="37" t="s">
+        <v>75</v>
+      </c>
+      <c r="J9" s="37" t="s">
+        <v>75</v>
+      </c>
+      <c r="K9" s="37" t="s">
+        <v>75</v>
+      </c>
+      <c r="L9" s="37" t="s">
+        <v>75</v>
+      </c>
+      <c r="M9" s="37" t="s">
+        <v>75</v>
+      </c>
+      <c r="N9" s="37" t="s">
+        <v>75</v>
+      </c>
+      <c r="O9" s="37" t="s">
+        <v>75</v>
+      </c>
+      <c r="P9" s="37" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q9" s="37" t="s">
+        <v>75</v>
+      </c>
+      <c r="R9" s="37" t="s">
+        <v>75</v>
+      </c>
+      <c r="S9" s="37" t="s">
+        <v>75</v>
+      </c>
+      <c r="T9" s="37" t="s">
+        <v>75</v>
+      </c>
+      <c r="U9" s="37" t="s">
+        <v>75</v>
+      </c>
+      <c r="V9" s="37" t="s">
+        <v>75</v>
+      </c>
+      <c r="W9" s="37" t="s">
+        <v>75</v>
+      </c>
+      <c r="X9" s="37" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y9" s="37" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z9" s="37" t="s">
+        <v>75</v>
+      </c>
+      <c r="AA9" s="37" t="s">
+        <v>75</v>
+      </c>
+      <c r="AB9" s="37" t="s">
+        <v>75</v>
+      </c>
+      <c r="AC9" s="37" t="s">
+        <v>75</v>
+      </c>
+      <c r="AD9" s="37" t="s">
+        <v>75</v>
+      </c>
+      <c r="AE9" s="37" t="s">
+        <v>75</v>
+      </c>
+      <c r="AF9" s="37" t="s">
+        <v>75</v>
+      </c>
+      <c r="AG9" s="73"/>
+      <c r="AH9" s="88"/>
+      <c r="AI9" s="89"/>
+      <c r="AJ9" s="89"/>
+      <c r="AK9" s="89"/>
+      <c r="AL9" s="89"/>
+      <c r="AM9" s="89"/>
+      <c r="AN9" s="90"/>
+      <c r="AO9" s="58"/>
     </row>
     <row r="10" spans="1:41" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="56"/>
-      <c r="B10" s="56"/>
-      <c r="C10" s="56"/>
-      <c r="D10" s="56"/>
-      <c r="E10" s="56"/>
-      <c r="F10" s="56"/>
-      <c r="G10" s="56"/>
-      <c r="H10" s="56"/>
-      <c r="I10" s="56"/>
-      <c r="J10" s="56"/>
-      <c r="K10" s="56"/>
-      <c r="L10" s="56"/>
-      <c r="M10" s="56"/>
-      <c r="N10" s="56"/>
-      <c r="O10" s="56"/>
-      <c r="P10" s="56"/>
-      <c r="Q10" s="56"/>
-      <c r="R10" s="56"/>
-      <c r="S10" s="56"/>
-      <c r="T10" s="56"/>
-      <c r="U10" s="56"/>
-      <c r="V10" s="56"/>
-      <c r="W10" s="56"/>
-      <c r="X10" s="56"/>
-      <c r="Y10" s="56"/>
-      <c r="Z10" s="56"/>
-      <c r="AA10" s="56"/>
-      <c r="AB10" s="56"/>
-      <c r="AC10" s="56"/>
-      <c r="AD10" s="56"/>
-      <c r="AE10" s="56"/>
-      <c r="AF10" s="56"/>
-      <c r="AG10" s="56"/>
-      <c r="AH10" s="57"/>
-      <c r="AI10" s="57"/>
-      <c r="AJ10" s="57"/>
-      <c r="AK10" s="57"/>
-      <c r="AL10" s="57"/>
-      <c r="AM10" s="57"/>
-      <c r="AN10" s="57"/>
-      <c r="AO10" s="56"/>
+      <c r="A10" s="47"/>
+      <c r="B10" s="47"/>
+      <c r="C10" s="47"/>
+      <c r="D10" s="47"/>
+      <c r="E10" s="47"/>
+      <c r="F10" s="47"/>
+      <c r="G10" s="47"/>
+      <c r="H10" s="47"/>
+      <c r="I10" s="47"/>
+      <c r="J10" s="47"/>
+      <c r="K10" s="47"/>
+      <c r="L10" s="47"/>
+      <c r="M10" s="47"/>
+      <c r="N10" s="47"/>
+      <c r="O10" s="47"/>
+      <c r="P10" s="47"/>
+      <c r="Q10" s="47"/>
+      <c r="R10" s="47"/>
+      <c r="S10" s="47"/>
+      <c r="T10" s="47"/>
+      <c r="U10" s="47"/>
+      <c r="V10" s="47"/>
+      <c r="W10" s="47"/>
+      <c r="X10" s="47"/>
+      <c r="Y10" s="47"/>
+      <c r="Z10" s="47"/>
+      <c r="AA10" s="47"/>
+      <c r="AB10" s="47"/>
+      <c r="AC10" s="47"/>
+      <c r="AD10" s="47"/>
+      <c r="AE10" s="47"/>
+      <c r="AF10" s="47"/>
+      <c r="AG10" s="47"/>
+      <c r="AH10" s="48"/>
+      <c r="AI10" s="48"/>
+      <c r="AJ10" s="48"/>
+      <c r="AK10" s="48"/>
+      <c r="AL10" s="48"/>
+      <c r="AM10" s="48"/>
+      <c r="AN10" s="48"/>
+      <c r="AO10" s="47"/>
     </row>
-    <row r="11" spans="1:41" s="22" customFormat="1" ht="14.85" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="58"/>
-      <c r="B11" s="121" t="s">
-        <v>75</v>
-      </c>
-      <c r="C11" s="121" t="e">
+    <row r="11" spans="1:41" s="21" customFormat="1" ht="14.85" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="49"/>
+      <c r="B11" s="57" t="s">
+        <v>67</v>
+      </c>
+      <c r="C11" s="120" t="e">
         <f>B$11+1</f>
         <v>#VALUE!</v>
       </c>
-      <c r="D11" s="121" t="e">
+      <c r="D11" s="120" t="e">
         <f t="shared" ref="D11:AF11" si="0">C$11+1</f>
         <v>#VALUE!</v>
       </c>
-      <c r="E11" s="121" t="e">
+      <c r="E11" s="120" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="F11" s="121" t="e">
+      <c r="F11" s="120" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="G11" s="121" t="e">
+      <c r="G11" s="120" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="H11" s="121" t="e">
+      <c r="H11" s="120" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="I11" s="121" t="e">
+      <c r="I11" s="120" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="J11" s="121" t="e">
+      <c r="J11" s="120" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="K11" s="121" t="e">
+      <c r="K11" s="120" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="L11" s="121" t="e">
+      <c r="L11" s="120" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="M11" s="121" t="e">
+      <c r="M11" s="120" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="N11" s="121" t="e">
+      <c r="N11" s="120" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="O11" s="121" t="e">
+      <c r="O11" s="120" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="P11" s="121" t="e">
+      <c r="P11" s="120" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="Q11" s="121" t="e">
+      <c r="Q11" s="120" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="R11" s="121" t="e">
+      <c r="R11" s="120" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="S11" s="121" t="e">
+      <c r="S11" s="120" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="T11" s="121" t="e">
+      <c r="T11" s="120" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="U11" s="121" t="e">
+      <c r="U11" s="120" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="V11" s="121" t="e">
+      <c r="V11" s="120" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="W11" s="121" t="e">
+      <c r="W11" s="120" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="X11" s="121" t="e">
+      <c r="X11" s="120" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="Y11" s="121" t="e">
+      <c r="Y11" s="120" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="Z11" s="121" t="e">
+      <c r="Z11" s="120" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="AA11" s="121" t="e">
+      <c r="AA11" s="120" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="AB11" s="121" t="e">
+      <c r="AB11" s="120" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="AC11" s="121" t="e">
+      <c r="AC11" s="120" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="AD11" s="121" t="e">
+      <c r="AD11" s="120" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="AE11" s="121" t="e">
+      <c r="AE11" s="120" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="AF11" s="121" t="e">
+      <c r="AF11" s="120" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="AG11" s="59" t="s">
+      <c r="AG11" s="50" t="s">
         <v>37</v>
       </c>
-      <c r="AH11" s="60" t="s">
+      <c r="AH11" s="51" t="s">
         <v>2</v>
       </c>
-      <c r="AI11" s="60" t="s">
+      <c r="AI11" s="51" t="s">
         <v>3</v>
       </c>
-      <c r="AJ11" s="61" t="s">
+      <c r="AJ11" s="52" t="s">
         <v>15</v>
       </c>
-      <c r="AK11" s="61" t="s">
+      <c r="AK11" s="52" t="s">
         <v>16</v>
       </c>
-      <c r="AL11" s="61" t="s">
+      <c r="AL11" s="52" t="s">
         <v>17</v>
       </c>
-      <c r="AM11" s="61" t="s">
+      <c r="AM11" s="52" t="s">
         <v>39</v>
       </c>
-      <c r="AN11" s="62" t="s">
-        <v>0</v>
-      </c>
-      <c r="AO11" s="63" t="s">
+      <c r="AN11" s="53" t="s">
+        <v>0</v>
+      </c>
+      <c r="AO11" s="54" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:41" s="22" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="70" t="s">
+    <row r="12" spans="1:41" s="21" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="91" t="s">
         <v>47</v>
       </c>
-      <c r="B12" s="64" t="s">
-        <v>67</v>
-      </c>
-      <c r="C12" s="64"/>
-      <c r="D12" s="64"/>
-      <c r="E12" s="64"/>
-      <c r="F12" s="64"/>
-      <c r="G12" s="64"/>
-      <c r="H12" s="64"/>
-      <c r="I12" s="64"/>
-      <c r="J12" s="64"/>
-      <c r="K12" s="64"/>
-      <c r="L12" s="64"/>
-      <c r="M12" s="64"/>
-      <c r="N12" s="64"/>
-      <c r="O12" s="64"/>
-      <c r="P12" s="64"/>
-      <c r="Q12" s="64"/>
-      <c r="R12" s="64"/>
-      <c r="S12" s="64"/>
-      <c r="T12" s="64"/>
-      <c r="U12" s="64"/>
-      <c r="V12" s="64"/>
-      <c r="W12" s="64"/>
-      <c r="X12" s="64"/>
-      <c r="Y12" s="64"/>
-      <c r="Z12" s="64"/>
-      <c r="AA12" s="64"/>
-      <c r="AB12" s="64"/>
-      <c r="AC12" s="64"/>
-      <c r="AD12" s="64"/>
-      <c r="AE12" s="64"/>
-      <c r="AF12" s="65"/>
+      <c r="B12" s="55" t="s">
+        <v>70</v>
+      </c>
+      <c r="C12" s="55" t="s">
+        <v>65</v>
+      </c>
+      <c r="D12" s="55" t="s">
+        <v>65</v>
+      </c>
+      <c r="E12" s="55" t="s">
+        <v>65</v>
+      </c>
+      <c r="F12" s="55" t="s">
+        <v>65</v>
+      </c>
+      <c r="G12" s="55" t="s">
+        <v>65</v>
+      </c>
+      <c r="H12" s="55" t="s">
+        <v>65</v>
+      </c>
+      <c r="I12" s="55" t="s">
+        <v>65</v>
+      </c>
+      <c r="J12" s="55" t="s">
+        <v>65</v>
+      </c>
+      <c r="K12" s="55" t="s">
+        <v>65</v>
+      </c>
+      <c r="L12" s="55" t="s">
+        <v>65</v>
+      </c>
+      <c r="M12" s="55" t="s">
+        <v>65</v>
+      </c>
+      <c r="N12" s="55" t="s">
+        <v>65</v>
+      </c>
+      <c r="O12" s="55" t="s">
+        <v>65</v>
+      </c>
+      <c r="P12" s="55" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q12" s="55" t="s">
+        <v>65</v>
+      </c>
+      <c r="R12" s="55" t="s">
+        <v>65</v>
+      </c>
+      <c r="S12" s="55" t="s">
+        <v>65</v>
+      </c>
+      <c r="T12" s="55" t="s">
+        <v>65</v>
+      </c>
+      <c r="U12" s="55" t="s">
+        <v>65</v>
+      </c>
+      <c r="V12" s="55" t="s">
+        <v>65</v>
+      </c>
+      <c r="W12" s="55" t="s">
+        <v>65</v>
+      </c>
+      <c r="X12" s="55" t="s">
+        <v>65</v>
+      </c>
+      <c r="Y12" s="55" t="s">
+        <v>65</v>
+      </c>
+      <c r="Z12" s="55" t="s">
+        <v>65</v>
+      </c>
+      <c r="AA12" s="55" t="s">
+        <v>65</v>
+      </c>
+      <c r="AB12" s="55" t="s">
+        <v>65</v>
+      </c>
+      <c r="AC12" s="55" t="s">
+        <v>65</v>
+      </c>
+      <c r="AD12" s="55" t="s">
+        <v>65</v>
+      </c>
+      <c r="AE12" s="55" t="s">
+        <v>65</v>
+      </c>
+      <c r="AF12" s="55" t="s">
+        <v>65</v>
+      </c>
       <c r="AG12" s="93"/>
-      <c r="AH12" s="72" t="s">
+      <c r="AH12" s="95" t="s">
         <v>41</v>
       </c>
-      <c r="AI12" s="74" t="s">
+      <c r="AI12" s="97" t="s">
         <v>40</v>
       </c>
-      <c r="AJ12" s="75" t="s">
+      <c r="AJ12" s="99" t="s">
         <v>42</v>
       </c>
-      <c r="AK12" s="68" t="s">
+      <c r="AK12" s="102" t="s">
         <v>43</v>
       </c>
-      <c r="AL12" s="66" t="s">
+      <c r="AL12" s="101" t="s">
         <v>44</v>
       </c>
-      <c r="AM12" s="66" t="s">
+      <c r="AM12" s="101" t="s">
         <v>45</v>
       </c>
-      <c r="AN12" s="68" t="s">
+      <c r="AN12" s="102" t="s">
         <v>46</v>
       </c>
-      <c r="AO12" s="82"/>
+      <c r="AO12" s="104"/>
     </row>
     <row r="13" spans="1:41" s="15" customFormat="1" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="71"/>
-      <c r="B13" s="23" t="s">
-        <v>68</v>
-      </c>
-      <c r="C13" s="23"/>
-      <c r="D13" s="23"/>
-      <c r="E13" s="23"/>
-      <c r="F13" s="23"/>
-      <c r="G13" s="23"/>
-      <c r="H13" s="23"/>
-      <c r="I13" s="23"/>
-      <c r="J13" s="23"/>
-      <c r="K13" s="23"/>
-      <c r="L13" s="23"/>
-      <c r="M13" s="23"/>
-      <c r="N13" s="23"/>
-      <c r="O13" s="23"/>
-      <c r="P13" s="23"/>
-      <c r="Q13" s="23"/>
-      <c r="R13" s="23"/>
-      <c r="S13" s="23"/>
-      <c r="T13" s="23"/>
-      <c r="U13" s="23"/>
-      <c r="V13" s="23"/>
-      <c r="W13" s="23"/>
-      <c r="X13" s="23"/>
-      <c r="Y13" s="23"/>
-      <c r="Z13" s="23"/>
-      <c r="AA13" s="23"/>
-      <c r="AB13" s="23"/>
-      <c r="AC13" s="23"/>
-      <c r="AD13" s="23"/>
-      <c r="AE13" s="23"/>
-      <c r="AF13" s="24"/>
+      <c r="A13" s="92"/>
+      <c r="B13" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="C13" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="D13" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="E13" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="F13" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="G13" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="H13" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="I13" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="J13" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="K13" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="L13" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="M13" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="N13" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="O13" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="P13" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q13" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="R13" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="S13" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="T13" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="U13" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="V13" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="W13" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="X13" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="Y13" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z13" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="AA13" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="AB13" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="AC13" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="AD13" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="AE13" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="AF13" s="22" t="s">
+        <v>66</v>
+      </c>
       <c r="AG13" s="94"/>
-      <c r="AH13" s="73"/>
-      <c r="AI13" s="67"/>
-      <c r="AJ13" s="76"/>
-      <c r="AK13" s="69"/>
-      <c r="AL13" s="67"/>
-      <c r="AM13" s="67"/>
-      <c r="AN13" s="69"/>
-      <c r="AO13" s="83"/>
+      <c r="AH13" s="96"/>
+      <c r="AI13" s="98"/>
+      <c r="AJ13" s="100"/>
+      <c r="AK13" s="103"/>
+      <c r="AL13" s="98"/>
+      <c r="AM13" s="98"/>
+      <c r="AN13" s="103"/>
+      <c r="AO13" s="105"/>
     </row>
     <row r="14" spans="1:41" s="17" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="25"/>
-      <c r="C14" s="25"/>
-      <c r="D14" s="25"/>
-      <c r="E14" s="25"/>
-      <c r="F14" s="25"/>
-      <c r="G14" s="25"/>
-      <c r="H14" s="25"/>
-      <c r="I14" s="25"/>
-      <c r="J14" s="25"/>
-      <c r="K14" s="25"/>
-      <c r="L14" s="25"/>
-      <c r="M14" s="25"/>
-      <c r="N14" s="25"/>
-      <c r="O14" s="25"/>
-      <c r="P14" s="25"/>
-      <c r="Q14" s="25"/>
-      <c r="R14" s="25"/>
-      <c r="S14" s="25"/>
-      <c r="T14" s="25"/>
-      <c r="U14" s="25"/>
-      <c r="V14" s="25"/>
-      <c r="W14" s="25"/>
-      <c r="X14" s="25"/>
-      <c r="Y14" s="25"/>
-      <c r="Z14" s="25"/>
-      <c r="AA14" s="25"/>
-      <c r="AB14" s="25"/>
-      <c r="AC14" s="25"/>
-      <c r="AD14" s="25"/>
-      <c r="AE14" s="25"/>
-      <c r="AF14" s="26"/>
-      <c r="AG14" s="84"/>
-      <c r="AH14" s="86"/>
-      <c r="AI14" s="88"/>
-      <c r="AJ14" s="88"/>
-      <c r="AK14" s="88"/>
-      <c r="AL14" s="88"/>
-      <c r="AM14" s="27"/>
-      <c r="AN14" s="90"/>
-      <c r="AO14" s="91"/>
+      <c r="B14" s="24"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="24"/>
+      <c r="H14" s="24"/>
+      <c r="I14" s="24"/>
+      <c r="J14" s="24"/>
+      <c r="K14" s="24"/>
+      <c r="L14" s="24"/>
+      <c r="M14" s="24"/>
+      <c r="N14" s="24"/>
+      <c r="O14" s="24"/>
+      <c r="P14" s="24"/>
+      <c r="Q14" s="24"/>
+      <c r="R14" s="24"/>
+      <c r="S14" s="24"/>
+      <c r="T14" s="24"/>
+      <c r="U14" s="24"/>
+      <c r="V14" s="24"/>
+      <c r="W14" s="24"/>
+      <c r="X14" s="24"/>
+      <c r="Y14" s="24"/>
+      <c r="Z14" s="24"/>
+      <c r="AA14" s="24"/>
+      <c r="AB14" s="24"/>
+      <c r="AC14" s="24"/>
+      <c r="AD14" s="24"/>
+      <c r="AE14" s="24"/>
+      <c r="AF14" s="25"/>
+      <c r="AG14" s="106"/>
+      <c r="AH14" s="108"/>
+      <c r="AI14" s="110"/>
+      <c r="AJ14" s="110"/>
+      <c r="AK14" s="110"/>
+      <c r="AL14" s="110"/>
+      <c r="AM14" s="63"/>
+      <c r="AN14" s="112"/>
+      <c r="AO14" s="113"/>
     </row>
     <row r="15" spans="1:41" s="17" customFormat="1" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="B15" s="28"/>
-      <c r="C15" s="28"/>
-      <c r="D15" s="28"/>
-      <c r="E15" s="28"/>
-      <c r="F15" s="28"/>
-      <c r="G15" s="28"/>
-      <c r="H15" s="28"/>
-      <c r="I15" s="28"/>
-      <c r="J15" s="28"/>
-      <c r="K15" s="28"/>
-      <c r="L15" s="28"/>
-      <c r="M15" s="28"/>
-      <c r="N15" s="28"/>
-      <c r="O15" s="28"/>
-      <c r="P15" s="28"/>
-      <c r="Q15" s="28"/>
-      <c r="R15" s="28"/>
-      <c r="S15" s="28"/>
-      <c r="T15" s="28"/>
-      <c r="U15" s="28"/>
-      <c r="V15" s="28"/>
-      <c r="W15" s="28"/>
-      <c r="X15" s="28"/>
-      <c r="Y15" s="28"/>
-      <c r="Z15" s="28"/>
-      <c r="AA15" s="28"/>
-      <c r="AB15" s="28"/>
-      <c r="AC15" s="28"/>
-      <c r="AD15" s="28"/>
-      <c r="AE15" s="28"/>
-      <c r="AF15" s="29"/>
-      <c r="AG15" s="85"/>
-      <c r="AH15" s="87"/>
-      <c r="AI15" s="89"/>
-      <c r="AJ15" s="89"/>
-      <c r="AK15" s="89"/>
-      <c r="AL15" s="89"/>
-      <c r="AM15" s="30"/>
-      <c r="AN15" s="89"/>
-      <c r="AO15" s="92"/>
+      <c r="B15" s="26"/>
+      <c r="C15" s="26"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="26"/>
+      <c r="F15" s="26"/>
+      <c r="G15" s="26"/>
+      <c r="H15" s="26"/>
+      <c r="I15" s="26"/>
+      <c r="J15" s="26"/>
+      <c r="K15" s="26"/>
+      <c r="L15" s="26"/>
+      <c r="M15" s="26"/>
+      <c r="N15" s="26"/>
+      <c r="O15" s="26"/>
+      <c r="P15" s="26"/>
+      <c r="Q15" s="26"/>
+      <c r="R15" s="26"/>
+      <c r="S15" s="26"/>
+      <c r="T15" s="26"/>
+      <c r="U15" s="26"/>
+      <c r="V15" s="26"/>
+      <c r="W15" s="26"/>
+      <c r="X15" s="26"/>
+      <c r="Y15" s="26"/>
+      <c r="Z15" s="26"/>
+      <c r="AA15" s="26"/>
+      <c r="AB15" s="26"/>
+      <c r="AC15" s="26"/>
+      <c r="AD15" s="26"/>
+      <c r="AE15" s="26"/>
+      <c r="AF15" s="27"/>
+      <c r="AG15" s="107"/>
+      <c r="AH15" s="109"/>
+      <c r="AI15" s="111"/>
+      <c r="AJ15" s="111"/>
+      <c r="AK15" s="111"/>
+      <c r="AL15" s="111"/>
+      <c r="AM15" s="62"/>
+      <c r="AN15" s="111"/>
+      <c r="AO15" s="114"/>
     </row>
     <row r="16" spans="1:41" s="15" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="70" t="s">
+      <c r="A16" s="91" t="s">
         <v>48</v>
       </c>
-      <c r="B16" s="64"/>
-      <c r="C16" s="64"/>
-      <c r="D16" s="64"/>
-      <c r="E16" s="64"/>
-      <c r="F16" s="64"/>
-      <c r="G16" s="64"/>
-      <c r="H16" s="64"/>
-      <c r="I16" s="64"/>
-      <c r="J16" s="64"/>
-      <c r="K16" s="64"/>
-      <c r="L16" s="64"/>
-      <c r="M16" s="64"/>
-      <c r="N16" s="64"/>
-      <c r="O16" s="64"/>
-      <c r="P16" s="64"/>
-      <c r="Q16" s="64"/>
-      <c r="R16" s="64"/>
-      <c r="S16" s="64"/>
-      <c r="T16" s="64"/>
-      <c r="U16" s="64"/>
-      <c r="V16" s="64"/>
-      <c r="W16" s="64"/>
-      <c r="X16" s="64"/>
-      <c r="Y16" s="64"/>
-      <c r="Z16" s="64"/>
-      <c r="AA16" s="64"/>
-      <c r="AB16" s="64"/>
-      <c r="AC16" s="64"/>
-      <c r="AD16" s="64"/>
-      <c r="AE16" s="64"/>
-      <c r="AF16" s="65"/>
+      <c r="B16" s="55"/>
+      <c r="C16" s="55"/>
+      <c r="D16" s="55"/>
+      <c r="E16" s="55"/>
+      <c r="F16" s="55"/>
+      <c r="G16" s="55"/>
+      <c r="H16" s="55"/>
+      <c r="I16" s="55"/>
+      <c r="J16" s="55"/>
+      <c r="K16" s="55"/>
+      <c r="L16" s="55"/>
+      <c r="M16" s="55"/>
+      <c r="N16" s="55"/>
+      <c r="O16" s="55"/>
+      <c r="P16" s="55"/>
+      <c r="Q16" s="55"/>
+      <c r="R16" s="55"/>
+      <c r="S16" s="55"/>
+      <c r="T16" s="55"/>
+      <c r="U16" s="55"/>
+      <c r="V16" s="55"/>
+      <c r="W16" s="55"/>
+      <c r="X16" s="55"/>
+      <c r="Y16" s="55"/>
+      <c r="Z16" s="55"/>
+      <c r="AA16" s="55"/>
+      <c r="AB16" s="55"/>
+      <c r="AC16" s="55"/>
+      <c r="AD16" s="55"/>
+      <c r="AE16" s="55"/>
+      <c r="AF16" s="56"/>
       <c r="AG16" s="93"/>
-      <c r="AH16" s="95"/>
-      <c r="AI16" s="80"/>
-      <c r="AJ16" s="80"/>
-      <c r="AK16" s="80"/>
-      <c r="AL16" s="97"/>
-      <c r="AM16" s="97"/>
-      <c r="AN16" s="80"/>
-      <c r="AO16" s="82"/>
+      <c r="AH16" s="115"/>
+      <c r="AI16" s="102"/>
+      <c r="AJ16" s="102"/>
+      <c r="AK16" s="102"/>
+      <c r="AL16" s="101"/>
+      <c r="AM16" s="101"/>
+      <c r="AN16" s="102"/>
+      <c r="AO16" s="104"/>
     </row>
     <row r="17" spans="1:41" s="15" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="71"/>
-      <c r="B17" s="23"/>
-      <c r="C17" s="23"/>
-      <c r="D17" s="23"/>
-      <c r="E17" s="23"/>
-      <c r="F17" s="23"/>
-      <c r="G17" s="23"/>
-      <c r="H17" s="23"/>
-      <c r="I17" s="23"/>
-      <c r="J17" s="23"/>
-      <c r="K17" s="23"/>
-      <c r="L17" s="23"/>
-      <c r="M17" s="23"/>
-      <c r="N17" s="23"/>
-      <c r="O17" s="23"/>
-      <c r="P17" s="23"/>
-      <c r="Q17" s="23"/>
-      <c r="R17" s="23"/>
-      <c r="S17" s="23"/>
-      <c r="T17" s="23"/>
-      <c r="U17" s="23"/>
-      <c r="V17" s="23"/>
-      <c r="W17" s="23"/>
-      <c r="X17" s="23"/>
-      <c r="Y17" s="23"/>
-      <c r="Z17" s="23"/>
-      <c r="AA17" s="23"/>
-      <c r="AB17" s="23"/>
-      <c r="AC17" s="23"/>
-      <c r="AD17" s="23"/>
-      <c r="AE17" s="23"/>
-      <c r="AF17" s="24"/>
+      <c r="A17" s="92"/>
+      <c r="B17" s="22"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="22"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="22"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="22"/>
+      <c r="K17" s="22"/>
+      <c r="L17" s="22"/>
+      <c r="M17" s="22"/>
+      <c r="N17" s="22"/>
+      <c r="O17" s="22"/>
+      <c r="P17" s="22"/>
+      <c r="Q17" s="22"/>
+      <c r="R17" s="22"/>
+      <c r="S17" s="22"/>
+      <c r="T17" s="22"/>
+      <c r="U17" s="22"/>
+      <c r="V17" s="22"/>
+      <c r="W17" s="22"/>
+      <c r="X17" s="22"/>
+      <c r="Y17" s="22"/>
+      <c r="Z17" s="22"/>
+      <c r="AA17" s="22"/>
+      <c r="AB17" s="22"/>
+      <c r="AC17" s="22"/>
+      <c r="AD17" s="22"/>
+      <c r="AE17" s="22"/>
+      <c r="AF17" s="23"/>
       <c r="AG17" s="94"/>
-      <c r="AH17" s="96"/>
-      <c r="AI17" s="81"/>
-      <c r="AJ17" s="81"/>
-      <c r="AK17" s="81"/>
+      <c r="AH17" s="116"/>
+      <c r="AI17" s="103"/>
+      <c r="AJ17" s="103"/>
+      <c r="AK17" s="103"/>
       <c r="AL17" s="98"/>
       <c r="AM17" s="98"/>
-      <c r="AN17" s="81"/>
-      <c r="AO17" s="83"/>
+      <c r="AN17" s="103"/>
+      <c r="AO17" s="105"/>
     </row>
     <row r="18" spans="1:41" s="17" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B18" s="25"/>
-      <c r="C18" s="25"/>
-      <c r="D18" s="25"/>
-      <c r="E18" s="25"/>
-      <c r="F18" s="25"/>
-      <c r="G18" s="25"/>
-      <c r="H18" s="25"/>
-      <c r="I18" s="25"/>
-      <c r="J18" s="25"/>
-      <c r="K18" s="25"/>
-      <c r="L18" s="25"/>
-      <c r="M18" s="25"/>
-      <c r="N18" s="25"/>
-      <c r="O18" s="25"/>
-      <c r="P18" s="25"/>
-      <c r="Q18" s="25"/>
-      <c r="R18" s="25"/>
-      <c r="S18" s="25"/>
-      <c r="T18" s="25"/>
-      <c r="U18" s="25"/>
-      <c r="V18" s="25"/>
-      <c r="W18" s="25"/>
-      <c r="X18" s="25"/>
-      <c r="Y18" s="25"/>
-      <c r="Z18" s="25"/>
-      <c r="AA18" s="25"/>
-      <c r="AB18" s="25"/>
-      <c r="AC18" s="25"/>
-      <c r="AD18" s="25"/>
-      <c r="AE18" s="25"/>
-      <c r="AF18" s="26"/>
-      <c r="AG18" s="84"/>
-      <c r="AH18" s="86"/>
-      <c r="AI18" s="88"/>
-      <c r="AJ18" s="88"/>
-      <c r="AK18" s="88"/>
-      <c r="AL18" s="88"/>
-      <c r="AM18" s="27"/>
-      <c r="AN18" s="90"/>
-      <c r="AO18" s="91"/>
+      <c r="B18" s="24"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="24"/>
+      <c r="E18" s="24"/>
+      <c r="F18" s="24"/>
+      <c r="G18" s="24"/>
+      <c r="H18" s="24"/>
+      <c r="I18" s="24"/>
+      <c r="J18" s="24"/>
+      <c r="K18" s="24"/>
+      <c r="L18" s="24"/>
+      <c r="M18" s="24"/>
+      <c r="N18" s="24"/>
+      <c r="O18" s="24"/>
+      <c r="P18" s="24"/>
+      <c r="Q18" s="24"/>
+      <c r="R18" s="24"/>
+      <c r="S18" s="24"/>
+      <c r="T18" s="24"/>
+      <c r="U18" s="24"/>
+      <c r="V18" s="24"/>
+      <c r="W18" s="24"/>
+      <c r="X18" s="24"/>
+      <c r="Y18" s="24"/>
+      <c r="Z18" s="24"/>
+      <c r="AA18" s="24"/>
+      <c r="AB18" s="24"/>
+      <c r="AC18" s="24"/>
+      <c r="AD18" s="24"/>
+      <c r="AE18" s="24"/>
+      <c r="AF18" s="25"/>
+      <c r="AG18" s="106"/>
+      <c r="AH18" s="108"/>
+      <c r="AI18" s="110"/>
+      <c r="AJ18" s="110"/>
+      <c r="AK18" s="110"/>
+      <c r="AL18" s="110"/>
+      <c r="AM18" s="63"/>
+      <c r="AN18" s="112"/>
+      <c r="AO18" s="113"/>
     </row>
     <row r="19" spans="1:41" s="17" customFormat="1" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="B19" s="28"/>
-      <c r="C19" s="28"/>
-      <c r="D19" s="28"/>
-      <c r="E19" s="28"/>
-      <c r="F19" s="28"/>
-      <c r="G19" s="28"/>
-      <c r="H19" s="28"/>
-      <c r="I19" s="28"/>
-      <c r="J19" s="28"/>
-      <c r="K19" s="28"/>
-      <c r="L19" s="28"/>
-      <c r="M19" s="28"/>
-      <c r="N19" s="28"/>
-      <c r="O19" s="28"/>
-      <c r="P19" s="28"/>
-      <c r="Q19" s="28"/>
-      <c r="R19" s="28"/>
-      <c r="S19" s="28"/>
-      <c r="T19" s="28"/>
-      <c r="U19" s="28"/>
-      <c r="V19" s="28"/>
-      <c r="W19" s="28"/>
-      <c r="X19" s="28"/>
-      <c r="Y19" s="28"/>
-      <c r="Z19" s="28"/>
-      <c r="AA19" s="28"/>
-      <c r="AB19" s="28"/>
-      <c r="AC19" s="28"/>
-      <c r="AD19" s="28"/>
-      <c r="AE19" s="28"/>
-      <c r="AF19" s="29"/>
-      <c r="AG19" s="85"/>
-      <c r="AH19" s="87"/>
-      <c r="AI19" s="89"/>
-      <c r="AJ19" s="89"/>
-      <c r="AK19" s="89"/>
-      <c r="AL19" s="89"/>
-      <c r="AM19" s="30"/>
-      <c r="AN19" s="89"/>
-      <c r="AO19" s="92"/>
+      <c r="B19" s="26"/>
+      <c r="C19" s="26"/>
+      <c r="D19" s="26"/>
+      <c r="E19" s="26"/>
+      <c r="F19" s="26"/>
+      <c r="G19" s="26"/>
+      <c r="H19" s="26"/>
+      <c r="I19" s="26"/>
+      <c r="J19" s="26"/>
+      <c r="K19" s="26"/>
+      <c r="L19" s="26"/>
+      <c r="M19" s="26"/>
+      <c r="N19" s="26"/>
+      <c r="O19" s="26"/>
+      <c r="P19" s="26"/>
+      <c r="Q19" s="26"/>
+      <c r="R19" s="26"/>
+      <c r="S19" s="26"/>
+      <c r="T19" s="26"/>
+      <c r="U19" s="26"/>
+      <c r="V19" s="26"/>
+      <c r="W19" s="26"/>
+      <c r="X19" s="26"/>
+      <c r="Y19" s="26"/>
+      <c r="Z19" s="26"/>
+      <c r="AA19" s="26"/>
+      <c r="AB19" s="26"/>
+      <c r="AC19" s="26"/>
+      <c r="AD19" s="26"/>
+      <c r="AE19" s="26"/>
+      <c r="AF19" s="27"/>
+      <c r="AG19" s="107"/>
+      <c r="AH19" s="109"/>
+      <c r="AI19" s="111"/>
+      <c r="AJ19" s="111"/>
+      <c r="AK19" s="111"/>
+      <c r="AL19" s="111"/>
+      <c r="AM19" s="62"/>
+      <c r="AN19" s="111"/>
+      <c r="AO19" s="114"/>
     </row>
     <row r="20" spans="1:41" s="17" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="122"/>
-      <c r="B20" s="123"/>
-      <c r="C20" s="123"/>
-      <c r="D20" s="123"/>
-      <c r="E20" s="123"/>
-      <c r="F20" s="123"/>
-      <c r="G20" s="123"/>
-      <c r="H20" s="123"/>
-      <c r="I20" s="123"/>
-      <c r="J20" s="123"/>
-      <c r="K20" s="123"/>
-      <c r="L20" s="123"/>
-      <c r="M20" s="123"/>
-      <c r="N20" s="123"/>
-      <c r="O20" s="123"/>
-      <c r="P20" s="123"/>
-      <c r="Q20" s="123"/>
-      <c r="R20" s="123"/>
-      <c r="S20" s="123"/>
-      <c r="T20" s="123"/>
-      <c r="U20" s="123"/>
-      <c r="V20" s="123"/>
-      <c r="W20" s="123"/>
-      <c r="X20" s="123"/>
-      <c r="Y20" s="123"/>
-      <c r="Z20" s="123"/>
-      <c r="AA20" s="123"/>
-      <c r="AB20" s="123"/>
-      <c r="AC20" s="123"/>
-      <c r="AD20" s="123"/>
-      <c r="AE20" s="123"/>
-      <c r="AF20" s="124"/>
-      <c r="AG20" s="124"/>
-      <c r="AH20" s="19"/>
-      <c r="AI20" s="19"/>
-      <c r="AJ20" s="19"/>
-      <c r="AK20" s="19"/>
-      <c r="AL20" s="19"/>
-      <c r="AM20" s="19"/>
-      <c r="AN20" s="19"/>
-      <c r="AO20" s="125"/>
+      <c r="A20" s="65"/>
+      <c r="B20" s="66"/>
+      <c r="C20" s="66"/>
+      <c r="D20" s="66"/>
+      <c r="E20" s="66"/>
+      <c r="F20" s="66"/>
+      <c r="G20" s="66"/>
+      <c r="H20" s="66"/>
+      <c r="I20" s="66"/>
+      <c r="J20" s="66"/>
+      <c r="K20" s="66"/>
+      <c r="L20" s="66"/>
+      <c r="M20" s="66"/>
+      <c r="N20" s="66"/>
+      <c r="O20" s="66"/>
+      <c r="P20" s="66"/>
+      <c r="Q20" s="66"/>
+      <c r="R20" s="66"/>
+      <c r="S20" s="66"/>
+      <c r="T20" s="66"/>
+      <c r="U20" s="66"/>
+      <c r="V20" s="66"/>
+      <c r="W20" s="66"/>
+      <c r="X20" s="66"/>
+      <c r="Y20" s="66"/>
+      <c r="Z20" s="66"/>
+      <c r="AA20" s="66"/>
+      <c r="AB20" s="66"/>
+      <c r="AC20" s="66"/>
+      <c r="AD20" s="66"/>
+      <c r="AE20" s="66"/>
+      <c r="AF20" s="67"/>
+      <c r="AG20" s="67"/>
+      <c r="AH20" s="30"/>
+      <c r="AI20" s="30"/>
+      <c r="AJ20" s="30"/>
+      <c r="AK20" s="30"/>
+      <c r="AL20" s="30"/>
+      <c r="AM20" s="30"/>
+      <c r="AN20" s="30"/>
+      <c r="AO20" s="68"/>
     </row>
     <row r="21" spans="1:41" s="17" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="122"/>
-      <c r="B21" s="123"/>
-      <c r="C21" s="123"/>
-      <c r="D21" s="123"/>
-      <c r="E21" s="123"/>
-      <c r="F21" s="123"/>
-      <c r="G21" s="123"/>
-      <c r="H21" s="123"/>
-      <c r="I21" s="123"/>
-      <c r="J21" s="123"/>
-      <c r="K21" s="123"/>
-      <c r="L21" s="123"/>
-      <c r="M21" s="123"/>
-      <c r="N21" s="123"/>
-      <c r="O21" s="123"/>
-      <c r="P21" s="123"/>
-      <c r="Q21" s="123"/>
-      <c r="R21" s="123"/>
-      <c r="S21" s="123"/>
-      <c r="T21" s="123"/>
-      <c r="U21" s="123"/>
-      <c r="V21" s="123"/>
-      <c r="W21" s="123"/>
-      <c r="X21" s="123"/>
-      <c r="Y21" s="123"/>
-      <c r="Z21" s="123"/>
-      <c r="AA21" s="123"/>
-      <c r="AB21" s="123"/>
-      <c r="AC21" s="123"/>
-      <c r="AD21" s="123"/>
-      <c r="AE21" s="123"/>
-      <c r="AF21" s="124"/>
-      <c r="AG21" s="124"/>
-      <c r="AH21" s="19"/>
-      <c r="AI21" s="19"/>
-      <c r="AJ21" s="19"/>
-      <c r="AK21" s="19"/>
-      <c r="AL21" s="19"/>
-      <c r="AM21" s="19"/>
-      <c r="AN21" s="19"/>
-      <c r="AO21" s="125"/>
+      <c r="A21" s="65"/>
+      <c r="B21" s="66"/>
+      <c r="C21" s="66"/>
+      <c r="D21" s="66"/>
+      <c r="E21" s="66"/>
+      <c r="F21" s="66"/>
+      <c r="G21" s="66"/>
+      <c r="H21" s="66"/>
+      <c r="I21" s="66"/>
+      <c r="J21" s="66"/>
+      <c r="K21" s="66"/>
+      <c r="L21" s="66"/>
+      <c r="M21" s="66"/>
+      <c r="N21" s="66"/>
+      <c r="O21" s="66"/>
+      <c r="P21" s="66"/>
+      <c r="Q21" s="66"/>
+      <c r="R21" s="66"/>
+      <c r="S21" s="66"/>
+      <c r="T21" s="66"/>
+      <c r="U21" s="66"/>
+      <c r="V21" s="66"/>
+      <c r="W21" s="66"/>
+      <c r="X21" s="66"/>
+      <c r="Y21" s="66"/>
+      <c r="Z21" s="66"/>
+      <c r="AA21" s="66"/>
+      <c r="AB21" s="66"/>
+      <c r="AC21" s="66"/>
+      <c r="AD21" s="66"/>
+      <c r="AE21" s="66"/>
+      <c r="AF21" s="67"/>
+      <c r="AG21" s="67"/>
+      <c r="AH21" s="30"/>
+      <c r="AI21" s="30"/>
+      <c r="AJ21" s="30"/>
+      <c r="AK21" s="30"/>
+      <c r="AL21" s="30"/>
+      <c r="AM21" s="30"/>
+      <c r="AN21" s="30"/>
+      <c r="AO21" s="68"/>
     </row>
     <row r="22" spans="1:41" s="17" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="122"/>
-      <c r="B22" s="123"/>
-      <c r="C22" s="123"/>
-      <c r="D22" s="123"/>
-      <c r="E22" s="123"/>
-      <c r="F22" s="123"/>
-      <c r="G22" s="123"/>
-      <c r="H22" s="123"/>
-      <c r="I22" s="123"/>
-      <c r="J22" s="123"/>
-      <c r="K22" s="123"/>
-      <c r="L22" s="123"/>
-      <c r="M22" s="123"/>
-      <c r="N22" s="123"/>
-      <c r="O22" s="123"/>
-      <c r="P22" s="123"/>
-      <c r="Q22" s="123"/>
-      <c r="R22" s="123"/>
-      <c r="S22" s="123"/>
-      <c r="T22" s="123"/>
-      <c r="U22" s="123"/>
-      <c r="V22" s="123"/>
-      <c r="W22" s="123"/>
-      <c r="X22" s="123"/>
-      <c r="Y22" s="123"/>
-      <c r="Z22" s="123"/>
-      <c r="AA22" s="123"/>
-      <c r="AB22" s="123"/>
-      <c r="AC22" s="123"/>
-      <c r="AD22" s="123"/>
-      <c r="AE22" s="123"/>
-      <c r="AF22" s="124"/>
-      <c r="AG22" s="124"/>
-      <c r="AH22" s="19"/>
-      <c r="AI22" s="19"/>
-      <c r="AJ22" s="19"/>
-      <c r="AK22" s="19"/>
-      <c r="AL22" s="19"/>
-      <c r="AM22" s="19"/>
-      <c r="AN22" s="19"/>
-      <c r="AO22" s="125"/>
+      <c r="A22" s="65"/>
+      <c r="B22" s="66"/>
+      <c r="C22" s="66"/>
+      <c r="D22" s="66"/>
+      <c r="E22" s="66"/>
+      <c r="F22" s="66"/>
+      <c r="G22" s="66"/>
+      <c r="H22" s="66"/>
+      <c r="I22" s="66"/>
+      <c r="J22" s="66"/>
+      <c r="K22" s="66"/>
+      <c r="L22" s="66"/>
+      <c r="M22" s="66"/>
+      <c r="N22" s="66"/>
+      <c r="O22" s="66"/>
+      <c r="P22" s="66"/>
+      <c r="Q22" s="66"/>
+      <c r="R22" s="66"/>
+      <c r="S22" s="66"/>
+      <c r="T22" s="66"/>
+      <c r="U22" s="66"/>
+      <c r="V22" s="66"/>
+      <c r="W22" s="66"/>
+      <c r="X22" s="66"/>
+      <c r="Y22" s="66"/>
+      <c r="Z22" s="66"/>
+      <c r="AA22" s="66"/>
+      <c r="AB22" s="66"/>
+      <c r="AC22" s="66"/>
+      <c r="AD22" s="66"/>
+      <c r="AE22" s="66"/>
+      <c r="AF22" s="67"/>
+      <c r="AG22" s="67"/>
+      <c r="AH22" s="30"/>
+      <c r="AI22" s="30"/>
+      <c r="AJ22" s="30"/>
+      <c r="AK22" s="30"/>
+      <c r="AL22" s="30"/>
+      <c r="AM22" s="30"/>
+      <c r="AN22" s="30"/>
+      <c r="AO22" s="68"/>
     </row>
     <row r="23" spans="1:41" s="17" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="122"/>
-      <c r="B23" s="123"/>
-      <c r="C23" s="123"/>
-      <c r="D23" s="123"/>
-      <c r="E23" s="123"/>
-      <c r="F23" s="123"/>
-      <c r="G23" s="123"/>
-      <c r="H23" s="123"/>
-      <c r="I23" s="123"/>
-      <c r="J23" s="123"/>
-      <c r="K23" s="123"/>
-      <c r="L23" s="123"/>
-      <c r="M23" s="123"/>
-      <c r="N23" s="123"/>
-      <c r="O23" s="123"/>
-      <c r="P23" s="123"/>
-      <c r="Q23" s="123"/>
-      <c r="R23" s="123"/>
-      <c r="S23" s="123"/>
-      <c r="T23" s="123"/>
-      <c r="U23" s="123"/>
-      <c r="V23" s="123"/>
-      <c r="W23" s="123"/>
-      <c r="X23" s="123"/>
-      <c r="Y23" s="123"/>
-      <c r="Z23" s="123"/>
-      <c r="AA23" s="123"/>
-      <c r="AB23" s="123"/>
-      <c r="AC23" s="123"/>
-      <c r="AD23" s="123"/>
-      <c r="AE23" s="123"/>
-      <c r="AF23" s="124"/>
-      <c r="AG23" s="124"/>
-      <c r="AH23" s="19"/>
-      <c r="AI23" s="19"/>
-      <c r="AJ23" s="19"/>
-      <c r="AK23" s="19"/>
-      <c r="AL23" s="19"/>
-      <c r="AM23" s="19"/>
-      <c r="AN23" s="19"/>
-      <c r="AO23" s="125"/>
+      <c r="A23" s="65"/>
+      <c r="B23" s="66"/>
+      <c r="C23" s="66"/>
+      <c r="D23" s="66"/>
+      <c r="E23" s="66"/>
+      <c r="F23" s="66"/>
+      <c r="G23" s="66"/>
+      <c r="H23" s="66"/>
+      <c r="I23" s="66"/>
+      <c r="J23" s="66"/>
+      <c r="K23" s="66"/>
+      <c r="L23" s="66"/>
+      <c r="M23" s="66"/>
+      <c r="N23" s="66"/>
+      <c r="O23" s="66"/>
+      <c r="P23" s="66"/>
+      <c r="Q23" s="66"/>
+      <c r="R23" s="66"/>
+      <c r="S23" s="66"/>
+      <c r="T23" s="66"/>
+      <c r="U23" s="66"/>
+      <c r="V23" s="66"/>
+      <c r="W23" s="66"/>
+      <c r="X23" s="66"/>
+      <c r="Y23" s="66"/>
+      <c r="Z23" s="66"/>
+      <c r="AA23" s="66"/>
+      <c r="AB23" s="66"/>
+      <c r="AC23" s="66"/>
+      <c r="AD23" s="66"/>
+      <c r="AE23" s="66"/>
+      <c r="AF23" s="67"/>
+      <c r="AG23" s="67"/>
+      <c r="AH23" s="30"/>
+      <c r="AI23" s="30"/>
+      <c r="AJ23" s="30"/>
+      <c r="AK23" s="30"/>
+      <c r="AL23" s="30"/>
+      <c r="AM23" s="30"/>
+      <c r="AN23" s="30"/>
+      <c r="AO23" s="68"/>
     </row>
     <row r="24" spans="1:41" s="15" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="31"/>
-      <c r="B24" s="32"/>
-      <c r="C24" s="32"/>
-      <c r="D24" s="32"/>
-      <c r="E24" s="32"/>
-      <c r="F24" s="32"/>
-      <c r="G24" s="32"/>
-      <c r="H24" s="32"/>
-      <c r="I24" s="32"/>
-      <c r="J24" s="32"/>
-      <c r="K24" s="32"/>
-      <c r="L24" s="32"/>
-      <c r="M24" s="32"/>
-      <c r="N24" s="32"/>
-      <c r="O24" s="32"/>
-      <c r="P24" s="32"/>
-      <c r="Q24" s="32"/>
-      <c r="R24" s="32"/>
-      <c r="S24" s="32"/>
-      <c r="T24" s="32"/>
-      <c r="U24" s="32"/>
-      <c r="V24" s="32"/>
-      <c r="W24" s="32"/>
-      <c r="X24" s="32"/>
-      <c r="Y24" s="32"/>
-      <c r="Z24" s="32"/>
-      <c r="AA24" s="32"/>
-      <c r="AB24" s="32"/>
-      <c r="AC24" s="32"/>
-      <c r="AD24" s="32"/>
-      <c r="AE24" s="32"/>
-      <c r="AF24" s="32"/>
-      <c r="AG24" s="32"/>
-      <c r="AH24" s="33"/>
-      <c r="AI24" s="33"/>
-      <c r="AJ24" s="33"/>
-      <c r="AK24" s="33"/>
-      <c r="AL24" s="33"/>
-      <c r="AM24" s="33"/>
-      <c r="AN24" s="33"/>
-      <c r="AO24" s="34"/>
+      <c r="A24" s="28"/>
+      <c r="B24" s="29"/>
+      <c r="C24" s="29"/>
+      <c r="D24" s="29"/>
+      <c r="E24" s="29"/>
+      <c r="F24" s="29"/>
+      <c r="G24" s="29"/>
+      <c r="H24" s="29"/>
+      <c r="I24" s="29"/>
+      <c r="J24" s="29"/>
+      <c r="K24" s="29"/>
+      <c r="L24" s="29"/>
+      <c r="M24" s="29"/>
+      <c r="N24" s="29"/>
+      <c r="O24" s="29"/>
+      <c r="P24" s="29"/>
+      <c r="Q24" s="29"/>
+      <c r="R24" s="29"/>
+      <c r="S24" s="29"/>
+      <c r="T24" s="29"/>
+      <c r="U24" s="29"/>
+      <c r="V24" s="29"/>
+      <c r="W24" s="29"/>
+      <c r="X24" s="29"/>
+      <c r="Y24" s="29"/>
+      <c r="Z24" s="29"/>
+      <c r="AA24" s="29"/>
+      <c r="AB24" s="29"/>
+      <c r="AC24" s="29"/>
+      <c r="AD24" s="29"/>
+      <c r="AE24" s="29"/>
+      <c r="AF24" s="29"/>
+      <c r="AG24" s="29"/>
+      <c r="AH24" s="30"/>
+      <c r="AI24" s="30"/>
+      <c r="AJ24" s="30"/>
+      <c r="AK24" s="30"/>
+      <c r="AL24" s="30"/>
+      <c r="AM24" s="30"/>
+      <c r="AN24" s="30"/>
+      <c r="AO24" s="31"/>
     </row>
     <row r="25" spans="1:41" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="35" t="s">
+      <c r="B25" s="64" t="s">
+        <v>50</v>
+      </c>
+      <c r="C25" s="117" t="s">
         <v>51</v>
       </c>
-      <c r="C25" s="77" t="s">
+      <c r="D25" s="117"/>
+      <c r="E25" s="117"/>
+      <c r="F25" s="32"/>
+      <c r="G25" s="32"/>
+      <c r="H25" s="64" t="s">
         <v>52</v>
       </c>
-      <c r="D25" s="77"/>
-      <c r="E25" s="77"/>
-      <c r="F25" s="36"/>
-      <c r="G25" s="36"/>
-      <c r="H25" s="35" t="s">
+      <c r="I25" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="I25" s="36" t="s">
+      <c r="J25" s="32"/>
+      <c r="K25" s="32"/>
+      <c r="L25" s="32"/>
+      <c r="N25" s="119" t="s">
         <v>54</v>
       </c>
-      <c r="J25" s="36"/>
-      <c r="K25" s="36"/>
-      <c r="L25" s="36"/>
-      <c r="N25" s="78" t="s">
+      <c r="O25" s="119"/>
+      <c r="P25" s="119"/>
+      <c r="Q25" s="119"/>
+      <c r="R25" s="119"/>
+      <c r="T25" s="119" t="s">
         <v>55</v>
       </c>
-      <c r="O25" s="78"/>
-      <c r="P25" s="78"/>
-      <c r="Q25" s="78"/>
-      <c r="R25" s="78"/>
-      <c r="T25" s="78" t="s">
+      <c r="U25" s="119"/>
+      <c r="V25" s="119"/>
+      <c r="W25" s="119"/>
+      <c r="X25" s="119"/>
+      <c r="Z25" s="33" t="s">
         <v>56</v>
       </c>
-      <c r="U25" s="78"/>
-      <c r="V25" s="78"/>
-      <c r="W25" s="78"/>
-      <c r="X25" s="78"/>
-      <c r="Z25" s="37" t="s">
-        <v>57</v>
-      </c>
-      <c r="AH25" s="20"/>
-      <c r="AI25" s="20"/>
-      <c r="AJ25" s="20"/>
-      <c r="AK25" s="20"/>
-      <c r="AL25" s="20"/>
-      <c r="AM25" s="20"/>
+      <c r="AH25" s="19"/>
+      <c r="AI25" s="19"/>
+      <c r="AJ25" s="19"/>
+      <c r="AK25" s="19"/>
+      <c r="AL25" s="19"/>
+      <c r="AM25" s="19"/>
     </row>
     <row r="26" spans="1:41" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B26" s="77" t="s">
-        <v>58</v>
-      </c>
-      <c r="C26" s="77"/>
-      <c r="D26" s="77"/>
-      <c r="E26" s="77"/>
-      <c r="F26" s="77"/>
-      <c r="G26" s="77"/>
-      <c r="H26" s="77"/>
-      <c r="I26" s="77"/>
-      <c r="J26" s="77"/>
-      <c r="K26" s="77"/>
-      <c r="L26" s="77"/>
-      <c r="M26" s="77"/>
-      <c r="N26" s="77"/>
-      <c r="O26" s="77"/>
-      <c r="P26" s="77"/>
-      <c r="Q26" s="77"/>
-      <c r="R26" s="77"/>
-      <c r="S26" s="77"/>
-      <c r="T26" s="77"/>
-      <c r="U26" s="77"/>
-      <c r="V26" s="77"/>
-      <c r="W26" s="77"/>
-      <c r="X26" s="77"/>
-      <c r="Y26" s="77"/>
-      <c r="Z26" s="77"/>
-      <c r="AA26" s="77"/>
-      <c r="AB26" s="77"/>
-      <c r="AC26" s="77"/>
-      <c r="AD26" s="77"/>
-      <c r="AE26" s="77"/>
-      <c r="AF26" s="77"/>
-      <c r="AG26" s="77"/>
-      <c r="AH26" s="77"/>
-      <c r="AI26" s="77"/>
-      <c r="AJ26" s="77"/>
-      <c r="AK26" s="77"/>
-      <c r="AL26" s="77"/>
-      <c r="AM26" s="77"/>
-      <c r="AN26" s="77"/>
-      <c r="AO26" s="77"/>
+      <c r="B26" s="117" t="s">
+        <v>57</v>
+      </c>
+      <c r="C26" s="117"/>
+      <c r="D26" s="117"/>
+      <c r="E26" s="117"/>
+      <c r="F26" s="117"/>
+      <c r="G26" s="117"/>
+      <c r="H26" s="117"/>
+      <c r="I26" s="117"/>
+      <c r="J26" s="117"/>
+      <c r="K26" s="117"/>
+      <c r="L26" s="117"/>
+      <c r="M26" s="117"/>
+      <c r="N26" s="117"/>
+      <c r="O26" s="117"/>
+      <c r="P26" s="117"/>
+      <c r="Q26" s="117"/>
+      <c r="R26" s="117"/>
+      <c r="S26" s="117"/>
+      <c r="T26" s="117"/>
+      <c r="U26" s="117"/>
+      <c r="V26" s="117"/>
+      <c r="W26" s="117"/>
+      <c r="X26" s="117"/>
+      <c r="Y26" s="117"/>
+      <c r="Z26" s="117"/>
+      <c r="AA26" s="117"/>
+      <c r="AB26" s="117"/>
+      <c r="AC26" s="117"/>
+      <c r="AD26" s="117"/>
+      <c r="AE26" s="117"/>
+      <c r="AF26" s="117"/>
+      <c r="AG26" s="117"/>
+      <c r="AH26" s="117"/>
+      <c r="AI26" s="117"/>
+      <c r="AJ26" s="117"/>
+      <c r="AK26" s="117"/>
+      <c r="AL26" s="117"/>
+      <c r="AM26" s="117"/>
+      <c r="AN26" s="117"/>
+      <c r="AO26" s="117"/>
     </row>
     <row r="27" spans="1:41" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="38"/>
-      <c r="B27" s="79" t="s">
-        <v>59</v>
-      </c>
-      <c r="C27" s="79"/>
-      <c r="D27" s="79"/>
-      <c r="E27" s="79"/>
-      <c r="F27" s="79"/>
-      <c r="G27" s="79"/>
-      <c r="H27" s="79"/>
-      <c r="I27" s="79"/>
-      <c r="J27" s="79"/>
-      <c r="K27" s="79"/>
-      <c r="L27" s="79"/>
-      <c r="M27" s="21"/>
-      <c r="N27" s="21"/>
-      <c r="O27" s="21"/>
-      <c r="P27" s="21"/>
-      <c r="Q27" s="21"/>
-      <c r="R27" s="21"/>
-      <c r="S27" s="21"/>
-      <c r="T27" s="21"/>
-      <c r="U27" s="21"/>
-      <c r="V27" s="21"/>
-      <c r="W27" s="21"/>
-      <c r="X27" s="21"/>
-      <c r="Y27" s="21"/>
-      <c r="Z27" s="21"/>
-      <c r="AA27" s="21"/>
-      <c r="AB27" s="21"/>
-      <c r="AC27" s="21"/>
-      <c r="AD27" s="21"/>
-      <c r="AH27" s="20"/>
-      <c r="AI27" s="20"/>
-      <c r="AJ27" s="20"/>
-      <c r="AK27" s="20"/>
-      <c r="AL27" s="20"/>
-      <c r="AM27" s="20"/>
+      <c r="A27" s="34"/>
+      <c r="B27" s="118" t="s">
+        <v>71</v>
+      </c>
+      <c r="C27" s="118"/>
+      <c r="D27" s="118"/>
+      <c r="E27" s="118"/>
+      <c r="F27" s="118"/>
+      <c r="G27" s="118"/>
+      <c r="H27" s="118"/>
+      <c r="I27" s="118"/>
+      <c r="J27" s="118"/>
+      <c r="K27" s="118"/>
+      <c r="L27" s="118"/>
+      <c r="M27" s="20"/>
+      <c r="N27" s="20"/>
+      <c r="O27" s="20"/>
+      <c r="P27" s="20"/>
+      <c r="Q27" s="20"/>
+      <c r="R27" s="20"/>
+      <c r="S27" s="20"/>
+      <c r="T27" s="20"/>
+      <c r="U27" s="20"/>
+      <c r="V27" s="20"/>
+      <c r="W27" s="20"/>
+      <c r="X27" s="20"/>
+      <c r="Y27" s="20"/>
+      <c r="Z27" s="20"/>
+      <c r="AA27" s="20"/>
+      <c r="AB27" s="20"/>
+      <c r="AC27" s="20"/>
+      <c r="AD27" s="20"/>
+      <c r="AH27" s="19"/>
+      <c r="AI27" s="19"/>
+      <c r="AJ27" s="19"/>
+      <c r="AK27" s="19"/>
+      <c r="AL27" s="19"/>
+      <c r="AM27" s="19"/>
     </row>
     <row r="28" spans="1:41" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="39"/>
-      <c r="B28" s="21"/>
-      <c r="C28" s="21"/>
-      <c r="D28" s="21"/>
-      <c r="E28" s="21"/>
-      <c r="F28" s="21"/>
-      <c r="G28" s="21"/>
-      <c r="H28" s="21"/>
-      <c r="I28" s="21"/>
-      <c r="J28" s="21" t="s">
+      <c r="A28" s="35"/>
+      <c r="B28" s="20"/>
+      <c r="C28" s="20"/>
+      <c r="D28" s="20"/>
+      <c r="E28" s="20"/>
+      <c r="F28" s="20"/>
+      <c r="G28" s="20"/>
+      <c r="H28" s="20"/>
+      <c r="I28" s="20"/>
+      <c r="J28" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="K28" s="20"/>
+      <c r="L28" s="20"/>
+      <c r="M28" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="N28" s="20"/>
+      <c r="O28" s="20"/>
+      <c r="P28" s="20"/>
+      <c r="Q28" s="20"/>
+      <c r="R28" s="20"/>
+      <c r="S28" s="20"/>
+      <c r="T28" s="20"/>
+      <c r="U28" s="20"/>
+      <c r="V28" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="K28" s="21"/>
-      <c r="L28" s="21"/>
-      <c r="M28" s="21" t="s">
+      <c r="W28" s="20"/>
+      <c r="X28" s="20"/>
+      <c r="Y28" s="20" t="s">
         <v>61</v>
       </c>
-      <c r="N28" s="21"/>
-      <c r="O28" s="21"/>
-      <c r="P28" s="21"/>
-      <c r="Q28" s="21"/>
-      <c r="R28" s="21"/>
-      <c r="S28" s="21"/>
-      <c r="T28" s="21"/>
-      <c r="U28" s="21"/>
-      <c r="V28" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="W28" s="21"/>
-      <c r="X28" s="21"/>
-      <c r="Y28" s="21" t="s">
-        <v>63</v>
-      </c>
-      <c r="Z28" s="21"/>
-      <c r="AA28" s="21"/>
-      <c r="AB28" s="21"/>
-      <c r="AC28" s="21"/>
-      <c r="AD28" s="21"/>
-      <c r="AH28" s="20"/>
-      <c r="AI28" s="20"/>
-      <c r="AJ28" s="20"/>
-      <c r="AK28" s="20"/>
-      <c r="AL28" s="20"/>
-      <c r="AM28" s="20"/>
+      <c r="Z28" s="20"/>
+      <c r="AA28" s="20"/>
+      <c r="AB28" s="20"/>
+      <c r="AC28" s="20"/>
+      <c r="AD28" s="20"/>
+      <c r="AH28" s="19"/>
+      <c r="AI28" s="19"/>
+      <c r="AJ28" s="19"/>
+      <c r="AK28" s="19"/>
+      <c r="AL28" s="19"/>
+      <c r="AM28" s="19"/>
     </row>
     <row r="29" spans="1:41" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B29" s="21"/>
-      <c r="C29" s="21"/>
-      <c r="D29" s="21"/>
-      <c r="E29" s="21"/>
-      <c r="F29" s="21"/>
-      <c r="G29" s="21"/>
-      <c r="H29" s="21"/>
-      <c r="I29" s="21"/>
-      <c r="J29" s="21"/>
-      <c r="K29" s="21"/>
-      <c r="L29" s="21"/>
-      <c r="M29" s="21" t="s">
-        <v>64</v>
-      </c>
-      <c r="N29" s="21"/>
-      <c r="O29" s="21"/>
-      <c r="P29" s="21"/>
-      <c r="Q29" s="21"/>
-      <c r="R29" s="21"/>
-      <c r="S29" s="21"/>
-      <c r="T29" s="21"/>
-      <c r="U29" s="21"/>
-      <c r="V29" s="21"/>
-      <c r="W29" s="21"/>
-      <c r="X29" s="21"/>
-      <c r="Y29" s="21" t="s">
-        <v>65</v>
-      </c>
-      <c r="Z29" s="21"/>
-      <c r="AA29" s="21"/>
-      <c r="AB29" s="21"/>
-      <c r="AC29" s="21"/>
-      <c r="AD29" s="21"/>
+      <c r="B29" s="20"/>
+      <c r="C29" s="20"/>
+      <c r="D29" s="20"/>
+      <c r="E29" s="20"/>
+      <c r="F29" s="20"/>
+      <c r="G29" s="20"/>
+      <c r="H29" s="20"/>
+      <c r="I29" s="20"/>
+      <c r="J29" s="20"/>
+      <c r="K29" s="20"/>
+      <c r="L29" s="20"/>
+      <c r="M29" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="N29" s="20"/>
+      <c r="O29" s="20"/>
+      <c r="P29" s="20"/>
+      <c r="Q29" s="20"/>
+      <c r="R29" s="20"/>
+      <c r="S29" s="20"/>
+      <c r="T29" s="20"/>
+      <c r="U29" s="20"/>
+      <c r="V29" s="20"/>
+      <c r="W29" s="20"/>
+      <c r="X29" s="20"/>
+      <c r="Y29" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="Z29" s="20"/>
+      <c r="AA29" s="20"/>
+      <c r="AB29" s="20"/>
+      <c r="AC29" s="20"/>
+      <c r="AD29" s="20"/>
     </row>
     <row r="30" spans="1:41" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B30" s="21"/>
-      <c r="C30" s="21"/>
-      <c r="D30" s="21"/>
-      <c r="E30" s="21"/>
-      <c r="F30" s="21"/>
-      <c r="G30" s="21"/>
-      <c r="H30" s="21"/>
-      <c r="I30" s="21"/>
-      <c r="J30" s="21"/>
-      <c r="K30" s="21"/>
-      <c r="L30" s="21"/>
-      <c r="M30" s="21"/>
-      <c r="N30" s="21"/>
-      <c r="O30" s="21"/>
-      <c r="P30" s="21"/>
-      <c r="Q30" s="21"/>
-      <c r="R30" s="21"/>
-      <c r="S30" s="21"/>
-      <c r="T30" s="21"/>
-      <c r="U30" s="21"/>
-      <c r="V30" s="21"/>
-      <c r="W30" s="21"/>
-      <c r="X30" s="21"/>
-      <c r="Y30" s="21"/>
-      <c r="Z30" s="21"/>
-      <c r="AA30" s="21"/>
-      <c r="AB30" s="21"/>
-      <c r="AC30" s="21"/>
-      <c r="AD30" s="21"/>
+      <c r="B30" s="20"/>
+      <c r="C30" s="20"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="20"/>
+      <c r="G30" s="20"/>
+      <c r="H30" s="20"/>
+      <c r="I30" s="20"/>
+      <c r="J30" s="20"/>
+      <c r="K30" s="20"/>
+      <c r="L30" s="20"/>
+      <c r="M30" s="20"/>
+      <c r="N30" s="20"/>
+      <c r="O30" s="20"/>
+      <c r="P30" s="20"/>
+      <c r="Q30" s="20"/>
+      <c r="R30" s="20"/>
+      <c r="S30" s="20"/>
+      <c r="T30" s="20"/>
+      <c r="U30" s="20"/>
+      <c r="V30" s="20"/>
+      <c r="W30" s="20"/>
+      <c r="X30" s="20"/>
+      <c r="Y30" s="20"/>
+      <c r="Z30" s="20"/>
+      <c r="AA30" s="20"/>
+      <c r="AB30" s="20"/>
+      <c r="AC30" s="20"/>
+      <c r="AD30" s="20"/>
     </row>
     <row r="31" spans="1:41" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B31" s="21" t="s">
-        <v>66</v>
-      </c>
-      <c r="C31" s="21"/>
-      <c r="D31" s="21"/>
-      <c r="E31" s="21"/>
-      <c r="F31" s="21"/>
-      <c r="G31" s="21"/>
-      <c r="H31" s="21"/>
-      <c r="I31" s="21"/>
-      <c r="J31" s="21"/>
-      <c r="K31" s="21"/>
-      <c r="L31" s="21"/>
-      <c r="M31" s="21"/>
-      <c r="N31" s="21"/>
-      <c r="O31" s="21"/>
-      <c r="P31" s="21"/>
-      <c r="Q31" s="21"/>
-      <c r="R31" s="21"/>
-      <c r="S31" s="21"/>
-      <c r="T31" s="21"/>
-      <c r="U31" s="21"/>
-      <c r="V31" s="21"/>
-      <c r="W31" s="21"/>
-      <c r="X31" s="21"/>
-      <c r="Y31" s="21"/>
-      <c r="Z31" s="21"/>
-      <c r="AA31" s="21"/>
-      <c r="AB31" s="21"/>
-      <c r="AC31" s="21"/>
-      <c r="AD31" s="21"/>
+      <c r="B31" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="C31" s="20"/>
+      <c r="D31" s="20"/>
+      <c r="E31" s="20"/>
+      <c r="F31" s="20"/>
+      <c r="G31" s="20"/>
+      <c r="H31" s="20"/>
+      <c r="I31" s="20"/>
+      <c r="J31" s="20"/>
+      <c r="K31" s="20"/>
+      <c r="L31" s="20"/>
+      <c r="M31" s="20"/>
+      <c r="N31" s="20"/>
+      <c r="O31" s="20"/>
+      <c r="P31" s="20"/>
+      <c r="Q31" s="20"/>
+      <c r="R31" s="20"/>
+      <c r="S31" s="20"/>
+      <c r="T31" s="20"/>
+      <c r="U31" s="20"/>
+      <c r="V31" s="20"/>
+      <c r="W31" s="20"/>
+      <c r="X31" s="20"/>
+      <c r="Y31" s="20"/>
+      <c r="Z31" s="20"/>
+      <c r="AA31" s="20"/>
+      <c r="AB31" s="20"/>
+      <c r="AC31" s="20"/>
+      <c r="AD31" s="20"/>
     </row>
     <row r="32" spans="1:41" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B32" s="21"/>
-      <c r="C32" s="21"/>
-      <c r="D32" s="21"/>
-      <c r="E32" s="21"/>
-      <c r="F32" s="21"/>
-      <c r="G32" s="21"/>
-      <c r="H32" s="21"/>
-      <c r="I32" s="21"/>
-      <c r="J32" s="21" t="s">
+      <c r="B32" s="20"/>
+      <c r="C32" s="20"/>
+      <c r="D32" s="20"/>
+      <c r="E32" s="20"/>
+      <c r="F32" s="20"/>
+      <c r="G32" s="20"/>
+      <c r="H32" s="20"/>
+      <c r="I32" s="20"/>
+      <c r="J32" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="K32" s="20"/>
+      <c r="L32" s="20"/>
+      <c r="M32" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="N32" s="20"/>
+      <c r="O32" s="20"/>
+      <c r="P32" s="20"/>
+      <c r="Q32" s="20"/>
+      <c r="R32" s="20"/>
+      <c r="S32" s="20"/>
+      <c r="T32" s="20"/>
+      <c r="U32" s="20"/>
+      <c r="V32" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="K32" s="21"/>
-      <c r="L32" s="21"/>
-      <c r="M32" s="21" t="s">
+      <c r="W32" s="20"/>
+      <c r="X32" s="20"/>
+      <c r="Y32" s="20" t="s">
         <v>61</v>
       </c>
-      <c r="N32" s="21"/>
-      <c r="O32" s="21"/>
-      <c r="P32" s="21"/>
-      <c r="Q32" s="21"/>
-      <c r="R32" s="21"/>
-      <c r="S32" s="21"/>
-      <c r="T32" s="21"/>
-      <c r="U32" s="21"/>
-      <c r="V32" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="W32" s="21"/>
-      <c r="X32" s="21"/>
-      <c r="Y32" s="21" t="s">
-        <v>63</v>
-      </c>
-      <c r="Z32" s="21"/>
-      <c r="AA32" s="21"/>
-      <c r="AB32" s="21"/>
-      <c r="AC32" s="21"/>
-      <c r="AD32" s="21"/>
+      <c r="Z32" s="20"/>
+      <c r="AA32" s="20"/>
+      <c r="AB32" s="20"/>
+      <c r="AC32" s="20"/>
+      <c r="AD32" s="20"/>
     </row>
     <row r="33" spans="2:30" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B33" s="21"/>
-      <c r="C33" s="21"/>
-      <c r="D33" s="21"/>
-      <c r="E33" s="21"/>
-      <c r="F33" s="21"/>
-      <c r="G33" s="21"/>
-      <c r="H33" s="21"/>
-      <c r="I33" s="21"/>
-      <c r="J33" s="21"/>
-      <c r="K33" s="21"/>
-      <c r="L33" s="21"/>
-      <c r="M33" s="21" t="s">
-        <v>64</v>
-      </c>
-      <c r="N33" s="21"/>
-      <c r="O33" s="21"/>
-      <c r="P33" s="21"/>
-      <c r="Q33" s="21"/>
-      <c r="R33" s="21"/>
-      <c r="S33" s="21"/>
-      <c r="T33" s="21"/>
-      <c r="U33" s="21"/>
-      <c r="V33" s="21"/>
-      <c r="W33" s="21"/>
-      <c r="X33" s="21"/>
-      <c r="Y33" s="21" t="s">
-        <v>65</v>
-      </c>
-      <c r="Z33" s="21"/>
-      <c r="AA33" s="21"/>
-      <c r="AB33" s="21"/>
-      <c r="AC33" s="21"/>
-      <c r="AD33" s="21"/>
+      <c r="B33" s="20"/>
+      <c r="C33" s="20"/>
+      <c r="D33" s="20"/>
+      <c r="E33" s="20"/>
+      <c r="F33" s="20"/>
+      <c r="G33" s="20"/>
+      <c r="H33" s="20"/>
+      <c r="I33" s="20"/>
+      <c r="J33" s="20"/>
+      <c r="K33" s="20"/>
+      <c r="L33" s="20"/>
+      <c r="M33" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="N33" s="20"/>
+      <c r="O33" s="20"/>
+      <c r="P33" s="20"/>
+      <c r="Q33" s="20"/>
+      <c r="R33" s="20"/>
+      <c r="S33" s="20"/>
+      <c r="T33" s="20"/>
+      <c r="U33" s="20"/>
+      <c r="V33" s="20"/>
+      <c r="W33" s="20"/>
+      <c r="X33" s="20"/>
+      <c r="Y33" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="Z33" s="20"/>
+      <c r="AA33" s="20"/>
+      <c r="AB33" s="20"/>
+      <c r="AC33" s="20"/>
+      <c r="AD33" s="20"/>
     </row>
     <row r="34" spans="2:30" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B34" s="21"/>
-      <c r="C34" s="21"/>
-      <c r="D34" s="21"/>
-      <c r="E34" s="21"/>
-      <c r="F34" s="21"/>
-      <c r="G34" s="21"/>
-      <c r="H34" s="21"/>
-      <c r="I34" s="21"/>
-      <c r="J34" s="21"/>
-      <c r="K34" s="21"/>
-      <c r="L34" s="21"/>
-      <c r="M34" s="21"/>
-      <c r="N34" s="21"/>
-      <c r="O34" s="21"/>
-      <c r="P34" s="21"/>
-      <c r="Q34" s="21"/>
-      <c r="R34" s="21"/>
-      <c r="S34" s="21"/>
-      <c r="T34" s="21"/>
-      <c r="U34" s="21"/>
-      <c r="V34" s="21"/>
-      <c r="W34" s="21"/>
-      <c r="X34" s="21"/>
-      <c r="Y34" s="21"/>
-      <c r="Z34" s="21"/>
-      <c r="AA34" s="21"/>
-      <c r="AB34" s="21"/>
-      <c r="AC34" s="21"/>
-      <c r="AD34" s="21"/>
+      <c r="B34" s="20"/>
+      <c r="C34" s="20"/>
+      <c r="D34" s="20"/>
+      <c r="E34" s="20"/>
+      <c r="F34" s="20"/>
+      <c r="G34" s="20"/>
+      <c r="H34" s="20"/>
+      <c r="I34" s="20"/>
+      <c r="J34" s="20"/>
+      <c r="K34" s="20"/>
+      <c r="L34" s="20"/>
+      <c r="M34" s="20"/>
+      <c r="N34" s="20"/>
+      <c r="O34" s="20"/>
+      <c r="P34" s="20"/>
+      <c r="Q34" s="20"/>
+      <c r="R34" s="20"/>
+      <c r="S34" s="20"/>
+      <c r="T34" s="20"/>
+      <c r="U34" s="20"/>
+      <c r="V34" s="20"/>
+      <c r="W34" s="20"/>
+      <c r="X34" s="20"/>
+      <c r="Y34" s="20"/>
+      <c r="Z34" s="20"/>
+      <c r="AA34" s="20"/>
+      <c r="AB34" s="20"/>
+      <c r="AC34" s="20"/>
+      <c r="AD34" s="20"/>
     </row>
     <row r="35" spans="2:30" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B35" s="21"/>
-      <c r="C35" s="21"/>
-      <c r="D35" s="21"/>
-      <c r="E35" s="21"/>
-      <c r="F35" s="21"/>
-      <c r="G35" s="21"/>
-      <c r="H35" s="21"/>
-      <c r="I35" s="21"/>
-      <c r="J35" s="21"/>
-      <c r="K35" s="21"/>
-      <c r="L35" s="21"/>
-      <c r="M35" s="21"/>
-      <c r="N35" s="21"/>
-      <c r="O35" s="21"/>
-      <c r="P35" s="21"/>
-      <c r="Q35" s="21"/>
-      <c r="R35" s="21"/>
-      <c r="S35" s="21"/>
-      <c r="T35" s="21"/>
-      <c r="U35" s="21"/>
-      <c r="V35" s="21"/>
-      <c r="W35" s="21"/>
-      <c r="X35" s="21"/>
-      <c r="Y35" s="21"/>
-      <c r="Z35" s="21"/>
-      <c r="AA35" s="21"/>
-      <c r="AB35" s="21"/>
-      <c r="AC35" s="21"/>
-      <c r="AD35" s="21"/>
+      <c r="B35" s="20"/>
+      <c r="C35" s="20"/>
+      <c r="D35" s="20"/>
+      <c r="E35" s="20"/>
+      <c r="F35" s="20"/>
+      <c r="G35" s="20"/>
+      <c r="H35" s="20"/>
+      <c r="I35" s="20"/>
+      <c r="J35" s="20"/>
+      <c r="K35" s="20"/>
+      <c r="L35" s="20"/>
+      <c r="M35" s="20"/>
+      <c r="N35" s="20"/>
+      <c r="O35" s="20"/>
+      <c r="P35" s="20"/>
+      <c r="Q35" s="20"/>
+      <c r="R35" s="20"/>
+      <c r="S35" s="20"/>
+      <c r="T35" s="20"/>
+      <c r="U35" s="20"/>
+      <c r="V35" s="20"/>
+      <c r="W35" s="20"/>
+      <c r="X35" s="20"/>
+      <c r="Y35" s="20"/>
+      <c r="Z35" s="20"/>
+      <c r="AA35" s="20"/>
+      <c r="AB35" s="20"/>
+      <c r="AC35" s="20"/>
+      <c r="AD35" s="20"/>
     </row>
     <row r="36" spans="2:30" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B36" s="21"/>
-      <c r="C36" s="21"/>
-      <c r="D36" s="21"/>
-      <c r="E36" s="21"/>
-      <c r="F36" s="21"/>
-      <c r="G36" s="21"/>
-      <c r="H36" s="21"/>
-      <c r="I36" s="21"/>
-      <c r="J36" s="21"/>
-      <c r="K36" s="21"/>
-      <c r="L36" s="21"/>
-      <c r="M36" s="21"/>
-      <c r="N36" s="21"/>
-      <c r="O36" s="21"/>
-      <c r="P36" s="21"/>
-      <c r="Q36" s="21"/>
-      <c r="R36" s="21"/>
-      <c r="S36" s="21"/>
-      <c r="T36" s="21"/>
-      <c r="U36" s="21"/>
-      <c r="V36" s="21"/>
-      <c r="W36" s="21"/>
-      <c r="X36" s="21"/>
-      <c r="Y36" s="21"/>
-      <c r="Z36" s="21"/>
-      <c r="AA36" s="21"/>
-      <c r="AB36" s="21"/>
-      <c r="AC36" s="21"/>
-      <c r="AD36" s="21"/>
+      <c r="B36" s="20"/>
+      <c r="C36" s="20"/>
+      <c r="D36" s="20"/>
+      <c r="E36" s="20"/>
+      <c r="F36" s="20"/>
+      <c r="G36" s="20"/>
+      <c r="H36" s="20"/>
+      <c r="I36" s="20"/>
+      <c r="J36" s="20"/>
+      <c r="K36" s="20"/>
+      <c r="L36" s="20"/>
+      <c r="M36" s="20"/>
+      <c r="N36" s="20"/>
+      <c r="O36" s="20"/>
+      <c r="P36" s="20"/>
+      <c r="Q36" s="20"/>
+      <c r="R36" s="20"/>
+      <c r="S36" s="20"/>
+      <c r="T36" s="20"/>
+      <c r="U36" s="20"/>
+      <c r="V36" s="20"/>
+      <c r="W36" s="20"/>
+      <c r="X36" s="20"/>
+      <c r="Y36" s="20"/>
+      <c r="Z36" s="20"/>
+      <c r="AA36" s="20"/>
+      <c r="AB36" s="20"/>
+      <c r="AC36" s="20"/>
+      <c r="AD36" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="50">
-    <mergeCell ref="A1:AO1"/>
-    <mergeCell ref="A2:AO2"/>
-    <mergeCell ref="A3:AO3"/>
-    <mergeCell ref="AG4:AG9"/>
-    <mergeCell ref="AH4:AL4"/>
-    <mergeCell ref="AO4:AO5"/>
-    <mergeCell ref="AH5:AN5"/>
-    <mergeCell ref="AH7:AL7"/>
-    <mergeCell ref="AH8:AN9"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="AG12:AG13"/>
-    <mergeCell ref="AH12:AH13"/>
-    <mergeCell ref="AI12:AI13"/>
-    <mergeCell ref="AJ12:AJ13"/>
+    <mergeCell ref="B26:AO26"/>
+    <mergeCell ref="B27:L27"/>
+    <mergeCell ref="AL18:AL19"/>
+    <mergeCell ref="AN18:AN19"/>
+    <mergeCell ref="AO18:AO19"/>
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="N25:R25"/>
+    <mergeCell ref="T25:X25"/>
+    <mergeCell ref="AG18:AG19"/>
+    <mergeCell ref="AH18:AH19"/>
+    <mergeCell ref="AI18:AI19"/>
+    <mergeCell ref="AJ18:AJ19"/>
+    <mergeCell ref="AK18:AK19"/>
+    <mergeCell ref="AK16:AK17"/>
+    <mergeCell ref="AL16:AL17"/>
+    <mergeCell ref="AM16:AM17"/>
+    <mergeCell ref="AN16:AN17"/>
+    <mergeCell ref="AO16:AO17"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="AG16:AG17"/>
+    <mergeCell ref="AH16:AH17"/>
+    <mergeCell ref="AI16:AI17"/>
+    <mergeCell ref="AJ16:AJ17"/>
     <mergeCell ref="AL12:AL13"/>
     <mergeCell ref="AM12:AM13"/>
     <mergeCell ref="AN12:AN13"/>
@@ -4155,40 +4618,23 @@
     <mergeCell ref="AK12:AK13"/>
     <mergeCell ref="AN14:AN15"/>
     <mergeCell ref="AO14:AO15"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="AG16:AG17"/>
-    <mergeCell ref="AH16:AH17"/>
-    <mergeCell ref="AI16:AI17"/>
-    <mergeCell ref="AJ16:AJ17"/>
-    <mergeCell ref="AK16:AK17"/>
-    <mergeCell ref="AL16:AL17"/>
-    <mergeCell ref="AM16:AM17"/>
-    <mergeCell ref="AN16:AN17"/>
-    <mergeCell ref="AO16:AO17"/>
-    <mergeCell ref="AG18:AG19"/>
-    <mergeCell ref="AH18:AH19"/>
-    <mergeCell ref="AI18:AI19"/>
-    <mergeCell ref="AJ18:AJ19"/>
-    <mergeCell ref="AK18:AK19"/>
-    <mergeCell ref="AL18:AL19"/>
-    <mergeCell ref="AN18:AN19"/>
-    <mergeCell ref="AO18:AO19"/>
-    <mergeCell ref="C25:E25"/>
-    <mergeCell ref="N25:R25"/>
-    <mergeCell ref="T25:X25"/>
-    <mergeCell ref="B26:AO26"/>
-    <mergeCell ref="B27:L27"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="AG12:AG13"/>
+    <mergeCell ref="AH12:AH13"/>
+    <mergeCell ref="AI12:AI13"/>
+    <mergeCell ref="AJ12:AJ13"/>
+    <mergeCell ref="A1:AO1"/>
+    <mergeCell ref="A2:AO2"/>
+    <mergeCell ref="A3:AO3"/>
+    <mergeCell ref="AG4:AG9"/>
+    <mergeCell ref="AH4:AL4"/>
+    <mergeCell ref="AO4:AO5"/>
+    <mergeCell ref="AH5:AN5"/>
+    <mergeCell ref="AH7:AL7"/>
+    <mergeCell ref="AH8:AN9"/>
   </mergeCells>
-  <conditionalFormatting sqref="B11:AF23">
-    <cfRule type="expression" dxfId="0" priority="2">
-      <formula>OR(WEEKDAY(D$11, 2)=6, WEEKDAY(D$11, 2)=7)</formula>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="75" fitToHeight="0" orientation="landscape" r:id="rId1"/>
-  <ignoredErrors>
-    <ignoredError sqref="D11:AF11" unlockedFormula="1"/>
-  </ignoredErrors>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Read excel file in main process, manipulate in renderer
</commit_message>
<xml_diff>
--- a/src/assets/template.xlsx
+++ b/src/assets/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Programming\scheduler\src\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CE8D8F6-FE13-4992-A00D-286BCDB91FDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE08B87D-D348-40F3-A040-030D5F056F70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -262,28 +262,28 @@
     <t xml:space="preserve"> ${year}. ${month} - Beosztás</t>
   </si>
   <si>
-    <t>${startsAt: [5]}</t>
-  </si>
-  <si>
     <t>${shiftStart: []}</t>
   </si>
   <si>
     <t>Mórahalom ${todayDate}</t>
   </si>
   <si>
-    <t>${startsAt: [7]}</t>
+    <t>${startsAt: 5}</t>
   </si>
   <si>
-    <t>${startsAt: [9]}</t>
+    <t>${startsAt: 7}</t>
   </si>
   <si>
-    <t>${startsAt: [11]}</t>
+    <t>${startsAt: 9}</t>
   </si>
   <si>
-    <t>${startsAt: [19]}</t>
+    <t>${startsAt: 11}</t>
   </si>
   <si>
-    <t>${presentBetween: [17,18]}</t>
+    <t>${presentBetween: 17, 18}</t>
+  </si>
+  <si>
+    <t>${startsAt: 19}</t>
   </si>
 </sst>
 </file>
@@ -1260,6 +1260,103 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="166" fontId="9" fillId="4" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="3" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="3" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="3" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="3" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="3" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="3" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="3" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="3" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="3" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="3" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
@@ -1326,103 +1423,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" fillId="3" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" fillId="3" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" fillId="3" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" fillId="3" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" fillId="3" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="3" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="3" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="3" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="3" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="3" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="9" fillId="4" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1864,7 +1864,7 @@
   <dimension ref="A1:AO36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="Y13" sqref="Y13"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2451,248 +2451,248 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:41" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="69" t="s">
+      <c r="A1" s="99" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="69"/>
-      <c r="C1" s="69"/>
-      <c r="D1" s="69"/>
-      <c r="E1" s="69"/>
-      <c r="F1" s="69"/>
-      <c r="G1" s="69"/>
-      <c r="H1" s="69"/>
-      <c r="I1" s="69"/>
-      <c r="J1" s="69"/>
-      <c r="K1" s="69"/>
-      <c r="L1" s="69"/>
-      <c r="M1" s="69"/>
-      <c r="N1" s="69"/>
-      <c r="O1" s="69"/>
-      <c r="P1" s="69"/>
-      <c r="Q1" s="69"/>
-      <c r="R1" s="69"/>
-      <c r="S1" s="69"/>
-      <c r="T1" s="69"/>
-      <c r="U1" s="69"/>
-      <c r="V1" s="69"/>
-      <c r="W1" s="69"/>
-      <c r="X1" s="69"/>
-      <c r="Y1" s="69"/>
-      <c r="Z1" s="69"/>
-      <c r="AA1" s="69"/>
-      <c r="AB1" s="69"/>
-      <c r="AC1" s="69"/>
-      <c r="AD1" s="69"/>
-      <c r="AE1" s="69"/>
-      <c r="AF1" s="69"/>
-      <c r="AG1" s="69"/>
-      <c r="AH1" s="69"/>
-      <c r="AI1" s="69"/>
-      <c r="AJ1" s="69"/>
-      <c r="AK1" s="69"/>
-      <c r="AL1" s="69"/>
-      <c r="AM1" s="69"/>
-      <c r="AN1" s="69"/>
-      <c r="AO1" s="69"/>
+      <c r="B1" s="99"/>
+      <c r="C1" s="99"/>
+      <c r="D1" s="99"/>
+      <c r="E1" s="99"/>
+      <c r="F1" s="99"/>
+      <c r="G1" s="99"/>
+      <c r="H1" s="99"/>
+      <c r="I1" s="99"/>
+      <c r="J1" s="99"/>
+      <c r="K1" s="99"/>
+      <c r="L1" s="99"/>
+      <c r="M1" s="99"/>
+      <c r="N1" s="99"/>
+      <c r="O1" s="99"/>
+      <c r="P1" s="99"/>
+      <c r="Q1" s="99"/>
+      <c r="R1" s="99"/>
+      <c r="S1" s="99"/>
+      <c r="T1" s="99"/>
+      <c r="U1" s="99"/>
+      <c r="V1" s="99"/>
+      <c r="W1" s="99"/>
+      <c r="X1" s="99"/>
+      <c r="Y1" s="99"/>
+      <c r="Z1" s="99"/>
+      <c r="AA1" s="99"/>
+      <c r="AB1" s="99"/>
+      <c r="AC1" s="99"/>
+      <c r="AD1" s="99"/>
+      <c r="AE1" s="99"/>
+      <c r="AF1" s="99"/>
+      <c r="AG1" s="99"/>
+      <c r="AH1" s="99"/>
+      <c r="AI1" s="99"/>
+      <c r="AJ1" s="99"/>
+      <c r="AK1" s="99"/>
+      <c r="AL1" s="99"/>
+      <c r="AM1" s="99"/>
+      <c r="AN1" s="99"/>
+      <c r="AO1" s="99"/>
     </row>
     <row r="2" spans="1:41" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="69" t="s">
+      <c r="A2" s="99" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="69"/>
-      <c r="C2" s="69"/>
-      <c r="D2" s="69"/>
-      <c r="E2" s="69"/>
-      <c r="F2" s="69"/>
-      <c r="G2" s="69"/>
-      <c r="H2" s="69"/>
-      <c r="I2" s="69"/>
-      <c r="J2" s="69"/>
-      <c r="K2" s="69"/>
-      <c r="L2" s="69"/>
-      <c r="M2" s="69"/>
-      <c r="N2" s="69"/>
-      <c r="O2" s="69"/>
-      <c r="P2" s="69"/>
-      <c r="Q2" s="69"/>
-      <c r="R2" s="69"/>
-      <c r="S2" s="69"/>
-      <c r="T2" s="69"/>
-      <c r="U2" s="69"/>
-      <c r="V2" s="69"/>
-      <c r="W2" s="69"/>
-      <c r="X2" s="69"/>
-      <c r="Y2" s="69"/>
-      <c r="Z2" s="69"/>
-      <c r="AA2" s="69"/>
-      <c r="AB2" s="69"/>
-      <c r="AC2" s="69"/>
-      <c r="AD2" s="69"/>
-      <c r="AE2" s="69"/>
-      <c r="AF2" s="69"/>
-      <c r="AG2" s="69"/>
-      <c r="AH2" s="69"/>
-      <c r="AI2" s="69"/>
-      <c r="AJ2" s="69"/>
-      <c r="AK2" s="69"/>
-      <c r="AL2" s="69"/>
-      <c r="AM2" s="69"/>
-      <c r="AN2" s="69"/>
-      <c r="AO2" s="69"/>
+      <c r="B2" s="99"/>
+      <c r="C2" s="99"/>
+      <c r="D2" s="99"/>
+      <c r="E2" s="99"/>
+      <c r="F2" s="99"/>
+      <c r="G2" s="99"/>
+      <c r="H2" s="99"/>
+      <c r="I2" s="99"/>
+      <c r="J2" s="99"/>
+      <c r="K2" s="99"/>
+      <c r="L2" s="99"/>
+      <c r="M2" s="99"/>
+      <c r="N2" s="99"/>
+      <c r="O2" s="99"/>
+      <c r="P2" s="99"/>
+      <c r="Q2" s="99"/>
+      <c r="R2" s="99"/>
+      <c r="S2" s="99"/>
+      <c r="T2" s="99"/>
+      <c r="U2" s="99"/>
+      <c r="V2" s="99"/>
+      <c r="W2" s="99"/>
+      <c r="X2" s="99"/>
+      <c r="Y2" s="99"/>
+      <c r="Z2" s="99"/>
+      <c r="AA2" s="99"/>
+      <c r="AB2" s="99"/>
+      <c r="AC2" s="99"/>
+      <c r="AD2" s="99"/>
+      <c r="AE2" s="99"/>
+      <c r="AF2" s="99"/>
+      <c r="AG2" s="99"/>
+      <c r="AH2" s="99"/>
+      <c r="AI2" s="99"/>
+      <c r="AJ2" s="99"/>
+      <c r="AK2" s="99"/>
+      <c r="AL2" s="99"/>
+      <c r="AM2" s="99"/>
+      <c r="AN2" s="99"/>
+      <c r="AO2" s="99"/>
     </row>
     <row r="3" spans="1:41" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="70" t="s">
+      <c r="A3" s="100" t="s">
         <v>49</v>
       </c>
-      <c r="B3" s="70"/>
-      <c r="C3" s="70"/>
-      <c r="D3" s="70"/>
-      <c r="E3" s="70"/>
-      <c r="F3" s="70"/>
-      <c r="G3" s="70"/>
-      <c r="H3" s="70"/>
-      <c r="I3" s="70"/>
-      <c r="J3" s="70"/>
-      <c r="K3" s="70"/>
-      <c r="L3" s="70"/>
-      <c r="M3" s="70"/>
-      <c r="N3" s="70"/>
-      <c r="O3" s="70"/>
-      <c r="P3" s="70"/>
-      <c r="Q3" s="70"/>
-      <c r="R3" s="70"/>
-      <c r="S3" s="70"/>
-      <c r="T3" s="70"/>
-      <c r="U3" s="70"/>
-      <c r="V3" s="70"/>
-      <c r="W3" s="70"/>
-      <c r="X3" s="70"/>
-      <c r="Y3" s="70"/>
-      <c r="Z3" s="70"/>
-      <c r="AA3" s="70"/>
-      <c r="AB3" s="70"/>
-      <c r="AC3" s="70"/>
-      <c r="AD3" s="70"/>
-      <c r="AE3" s="70"/>
-      <c r="AF3" s="70"/>
-      <c r="AG3" s="70"/>
-      <c r="AH3" s="70"/>
-      <c r="AI3" s="70"/>
-      <c r="AJ3" s="70"/>
-      <c r="AK3" s="70"/>
-      <c r="AL3" s="70"/>
-      <c r="AM3" s="70"/>
-      <c r="AN3" s="70"/>
-      <c r="AO3" s="70"/>
+      <c r="B3" s="100"/>
+      <c r="C3" s="100"/>
+      <c r="D3" s="100"/>
+      <c r="E3" s="100"/>
+      <c r="F3" s="100"/>
+      <c r="G3" s="100"/>
+      <c r="H3" s="100"/>
+      <c r="I3" s="100"/>
+      <c r="J3" s="100"/>
+      <c r="K3" s="100"/>
+      <c r="L3" s="100"/>
+      <c r="M3" s="100"/>
+      <c r="N3" s="100"/>
+      <c r="O3" s="100"/>
+      <c r="P3" s="100"/>
+      <c r="Q3" s="100"/>
+      <c r="R3" s="100"/>
+      <c r="S3" s="100"/>
+      <c r="T3" s="100"/>
+      <c r="U3" s="100"/>
+      <c r="V3" s="100"/>
+      <c r="W3" s="100"/>
+      <c r="X3" s="100"/>
+      <c r="Y3" s="100"/>
+      <c r="Z3" s="100"/>
+      <c r="AA3" s="100"/>
+      <c r="AB3" s="100"/>
+      <c r="AC3" s="100"/>
+      <c r="AD3" s="100"/>
+      <c r="AE3" s="100"/>
+      <c r="AF3" s="100"/>
+      <c r="AG3" s="100"/>
+      <c r="AH3" s="100"/>
+      <c r="AI3" s="100"/>
+      <c r="AJ3" s="100"/>
+      <c r="AK3" s="100"/>
+      <c r="AL3" s="100"/>
+      <c r="AM3" s="100"/>
+      <c r="AN3" s="100"/>
+      <c r="AO3" s="100"/>
     </row>
     <row r="4" spans="1:41" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="36" t="s">
         <v>21</v>
       </c>
       <c r="B4" s="37" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C4" s="37" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D4" s="37" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E4" s="37" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F4" s="37" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="G4" s="37" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="H4" s="37" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="I4" s="37" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="J4" s="37" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="K4" s="37" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="L4" s="37" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="M4" s="37" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="N4" s="37" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="O4" s="37" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="P4" s="37" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="Q4" s="37" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="R4" s="37" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="S4" s="37" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="T4" s="37" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="U4" s="37" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="V4" s="37" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="W4" s="37" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="X4" s="37" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="Y4" s="37" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="Z4" s="37" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="AA4" s="37" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="AB4" s="37" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="AC4" s="37" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="AD4" s="37" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="AE4" s="37" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="AF4" s="37" t="s">
-        <v>69</v>
-      </c>
-      <c r="AG4" s="71"/>
-      <c r="AH4" s="74" t="s">
+        <v>71</v>
+      </c>
+      <c r="AG4" s="101"/>
+      <c r="AH4" s="104" t="s">
         <v>28</v>
       </c>
-      <c r="AI4" s="75"/>
-      <c r="AJ4" s="75"/>
-      <c r="AK4" s="75"/>
-      <c r="AL4" s="76"/>
+      <c r="AI4" s="105"/>
+      <c r="AJ4" s="105"/>
+      <c r="AK4" s="105"/>
+      <c r="AL4" s="106"/>
       <c r="AM4" s="38"/>
       <c r="AN4" s="39"/>
-      <c r="AO4" s="77" t="s">
+      <c r="AO4" s="107" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2793,15 +2793,15 @@
       <c r="AF5" s="37" t="s">
         <v>72</v>
       </c>
-      <c r="AG5" s="72"/>
-      <c r="AH5" s="79"/>
-      <c r="AI5" s="80"/>
-      <c r="AJ5" s="80"/>
-      <c r="AK5" s="80"/>
-      <c r="AL5" s="80"/>
-      <c r="AM5" s="80"/>
-      <c r="AN5" s="81"/>
-      <c r="AO5" s="78"/>
+      <c r="AG5" s="102"/>
+      <c r="AH5" s="109"/>
+      <c r="AI5" s="110"/>
+      <c r="AJ5" s="110"/>
+      <c r="AK5" s="110"/>
+      <c r="AL5" s="110"/>
+      <c r="AM5" s="110"/>
+      <c r="AN5" s="111"/>
+      <c r="AO5" s="108"/>
     </row>
     <row r="6" spans="1:41" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="40" t="s">
@@ -2900,7 +2900,7 @@
       <c r="AF6" s="37" t="s">
         <v>73</v>
       </c>
-      <c r="AG6" s="72"/>
+      <c r="AG6" s="102"/>
       <c r="AH6" s="59"/>
       <c r="AI6" s="60"/>
       <c r="AJ6" s="60"/>
@@ -3009,14 +3009,14 @@
       <c r="AF7" s="37" t="s">
         <v>74</v>
       </c>
-      <c r="AG7" s="72"/>
-      <c r="AH7" s="82" t="s">
+      <c r="AG7" s="102"/>
+      <c r="AH7" s="112" t="s">
         <v>29</v>
       </c>
-      <c r="AI7" s="83"/>
-      <c r="AJ7" s="83"/>
-      <c r="AK7" s="83"/>
-      <c r="AL7" s="84"/>
+      <c r="AI7" s="113"/>
+      <c r="AJ7" s="113"/>
+      <c r="AK7" s="113"/>
+      <c r="AL7" s="114"/>
       <c r="AM7" s="43"/>
       <c r="AN7" s="44"/>
       <c r="AO7" s="45"/>
@@ -3026,106 +3026,106 @@
         <v>18</v>
       </c>
       <c r="B8" s="41" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C8" s="41" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D8" s="41" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E8" s="41" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F8" s="41" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G8" s="41" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H8" s="41" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I8" s="41" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J8" s="41" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K8" s="41" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="L8" s="41" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="M8" s="41" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="N8" s="41" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="O8" s="41" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="P8" s="41" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Q8" s="41" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="R8" s="41" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="S8" s="41" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="T8" s="41" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="U8" s="41" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="V8" s="41" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="W8" s="41" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="X8" s="41" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Y8" s="41" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Z8" s="41" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="AA8" s="41" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="AB8" s="41" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="AC8" s="41" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="AD8" s="41" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="AE8" s="41" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="AF8" s="41" t="s">
-        <v>76</v>
-      </c>
-      <c r="AG8" s="72"/>
-      <c r="AH8" s="85"/>
-      <c r="AI8" s="86"/>
-      <c r="AJ8" s="86"/>
-      <c r="AK8" s="86"/>
-      <c r="AL8" s="86"/>
-      <c r="AM8" s="86"/>
-      <c r="AN8" s="87"/>
+        <v>75</v>
+      </c>
+      <c r="AG8" s="102"/>
+      <c r="AH8" s="115"/>
+      <c r="AI8" s="116"/>
+      <c r="AJ8" s="116"/>
+      <c r="AK8" s="116"/>
+      <c r="AL8" s="116"/>
+      <c r="AM8" s="116"/>
+      <c r="AN8" s="117"/>
       <c r="AO8" s="45"/>
     </row>
     <row r="9" spans="1:41" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -3133,106 +3133,106 @@
         <v>24</v>
       </c>
       <c r="B9" s="37" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C9" s="37" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D9" s="37" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E9" s="37" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F9" s="37" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G9" s="37" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H9" s="37" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I9" s="37" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="J9" s="37" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="K9" s="37" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="L9" s="37" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="M9" s="37" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="N9" s="37" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="O9" s="37" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="P9" s="37" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="Q9" s="37" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="R9" s="37" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="S9" s="37" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="T9" s="37" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="U9" s="37" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="V9" s="37" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="W9" s="37" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="X9" s="37" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="Y9" s="37" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="Z9" s="37" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="AA9" s="37" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="AB9" s="37" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="AC9" s="37" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="AD9" s="37" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="AE9" s="37" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="AF9" s="37" t="s">
-        <v>75</v>
-      </c>
-      <c r="AG9" s="73"/>
-      <c r="AH9" s="88"/>
-      <c r="AI9" s="89"/>
-      <c r="AJ9" s="89"/>
-      <c r="AK9" s="89"/>
-      <c r="AL9" s="89"/>
-      <c r="AM9" s="89"/>
-      <c r="AN9" s="90"/>
+        <v>76</v>
+      </c>
+      <c r="AG9" s="103"/>
+      <c r="AH9" s="118"/>
+      <c r="AI9" s="119"/>
+      <c r="AJ9" s="119"/>
+      <c r="AK9" s="119"/>
+      <c r="AL9" s="119"/>
+      <c r="AM9" s="119"/>
+      <c r="AN9" s="120"/>
       <c r="AO9" s="58"/>
     </row>
     <row r="10" spans="1:41" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -3283,123 +3283,123 @@
       <c r="B11" s="57" t="s">
         <v>67</v>
       </c>
-      <c r="C11" s="120" t="e">
-        <f>B$11+1</f>
+      <c r="C11" s="69" t="e">
+        <f>B$11 + 1</f>
         <v>#VALUE!</v>
       </c>
-      <c r="D11" s="120" t="e">
-        <f t="shared" ref="D11:AF11" si="0">C$11+1</f>
+      <c r="D11" s="69" t="e">
+        <f t="shared" ref="D11:AF11" si="0">C$11 + 1</f>
         <v>#VALUE!</v>
       </c>
-      <c r="E11" s="120" t="e">
+      <c r="E11" s="69" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="F11" s="120" t="e">
+      <c r="F11" s="69" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="G11" s="120" t="e">
+      <c r="G11" s="69" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="H11" s="120" t="e">
+      <c r="H11" s="69" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="I11" s="120" t="e">
+      <c r="I11" s="69" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="J11" s="120" t="e">
+      <c r="J11" s="69" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="K11" s="120" t="e">
+      <c r="K11" s="69" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="L11" s="120" t="e">
+      <c r="L11" s="69" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="M11" s="120" t="e">
+      <c r="M11" s="69" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="N11" s="120" t="e">
+      <c r="N11" s="69" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="O11" s="120" t="e">
+      <c r="O11" s="69" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="P11" s="120" t="e">
+      <c r="P11" s="69" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="Q11" s="120" t="e">
+      <c r="Q11" s="69" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="R11" s="120" t="e">
+      <c r="R11" s="69" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="S11" s="120" t="e">
+      <c r="S11" s="69" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="T11" s="120" t="e">
+      <c r="T11" s="69" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="U11" s="120" t="e">
+      <c r="U11" s="69" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="V11" s="120" t="e">
+      <c r="V11" s="69" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="W11" s="120" t="e">
+      <c r="W11" s="69" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="X11" s="120" t="e">
+      <c r="X11" s="69" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="Y11" s="120" t="e">
+      <c r="Y11" s="69" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="Z11" s="120" t="e">
+      <c r="Z11" s="69" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="AA11" s="120" t="e">
+      <c r="AA11" s="69" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="AB11" s="120" t="e">
+      <c r="AB11" s="69" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="AC11" s="120" t="e">
+      <c r="AC11" s="69" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="AD11" s="120" t="e">
+      <c r="AD11" s="69" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="AE11" s="120" t="e">
+      <c r="AE11" s="69" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="AF11" s="120" t="e">
+      <c r="AF11" s="69" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
@@ -3432,11 +3432,11 @@
       </c>
     </row>
     <row r="12" spans="1:41" s="21" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="91" t="s">
+      <c r="A12" s="88" t="s">
         <v>47</v>
       </c>
       <c r="B12" s="55" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C12" s="55" t="s">
         <v>65</v>
@@ -3528,32 +3528,32 @@
       <c r="AF12" s="55" t="s">
         <v>65</v>
       </c>
-      <c r="AG12" s="93"/>
-      <c r="AH12" s="95" t="s">
+      <c r="AG12" s="90"/>
+      <c r="AH12" s="94" t="s">
         <v>41</v>
       </c>
-      <c r="AI12" s="97" t="s">
+      <c r="AI12" s="96" t="s">
         <v>40</v>
       </c>
-      <c r="AJ12" s="99" t="s">
+      <c r="AJ12" s="97" t="s">
         <v>42</v>
       </c>
-      <c r="AK12" s="102" t="s">
+      <c r="AK12" s="82" t="s">
         <v>43</v>
       </c>
-      <c r="AL12" s="101" t="s">
+      <c r="AL12" s="84" t="s">
         <v>44</v>
       </c>
-      <c r="AM12" s="101" t="s">
+      <c r="AM12" s="84" t="s">
         <v>45</v>
       </c>
-      <c r="AN12" s="102" t="s">
+      <c r="AN12" s="82" t="s">
         <v>46</v>
       </c>
-      <c r="AO12" s="104"/>
+      <c r="AO12" s="86"/>
     </row>
     <row r="13" spans="1:41" s="15" customFormat="1" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="92"/>
+      <c r="A13" s="89"/>
       <c r="B13" s="22" t="s">
         <v>66</v>
       </c>
@@ -3647,15 +3647,15 @@
       <c r="AF13" s="22" t="s">
         <v>66</v>
       </c>
-      <c r="AG13" s="94"/>
-      <c r="AH13" s="96"/>
-      <c r="AI13" s="98"/>
-      <c r="AJ13" s="100"/>
-      <c r="AK13" s="103"/>
-      <c r="AL13" s="98"/>
-      <c r="AM13" s="98"/>
-      <c r="AN13" s="103"/>
-      <c r="AO13" s="105"/>
+      <c r="AG13" s="91"/>
+      <c r="AH13" s="95"/>
+      <c r="AI13" s="85"/>
+      <c r="AJ13" s="98"/>
+      <c r="AK13" s="83"/>
+      <c r="AL13" s="85"/>
+      <c r="AM13" s="85"/>
+      <c r="AN13" s="83"/>
+      <c r="AO13" s="87"/>
     </row>
     <row r="14" spans="1:41" s="17" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
@@ -3692,15 +3692,15 @@
       <c r="AD14" s="24"/>
       <c r="AE14" s="24"/>
       <c r="AF14" s="25"/>
-      <c r="AG14" s="106"/>
-      <c r="AH14" s="108"/>
-      <c r="AI14" s="110"/>
-      <c r="AJ14" s="110"/>
-      <c r="AK14" s="110"/>
-      <c r="AL14" s="110"/>
+      <c r="AG14" s="78"/>
+      <c r="AH14" s="80"/>
+      <c r="AI14" s="72"/>
+      <c r="AJ14" s="72"/>
+      <c r="AK14" s="72"/>
+      <c r="AL14" s="72"/>
       <c r="AM14" s="63"/>
-      <c r="AN14" s="112"/>
-      <c r="AO14" s="113"/>
+      <c r="AN14" s="74"/>
+      <c r="AO14" s="75"/>
     </row>
     <row r="15" spans="1:41" s="17" customFormat="1" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
@@ -3737,18 +3737,18 @@
       <c r="AD15" s="26"/>
       <c r="AE15" s="26"/>
       <c r="AF15" s="27"/>
-      <c r="AG15" s="107"/>
-      <c r="AH15" s="109"/>
-      <c r="AI15" s="111"/>
-      <c r="AJ15" s="111"/>
-      <c r="AK15" s="111"/>
-      <c r="AL15" s="111"/>
+      <c r="AG15" s="79"/>
+      <c r="AH15" s="81"/>
+      <c r="AI15" s="73"/>
+      <c r="AJ15" s="73"/>
+      <c r="AK15" s="73"/>
+      <c r="AL15" s="73"/>
       <c r="AM15" s="62"/>
-      <c r="AN15" s="111"/>
-      <c r="AO15" s="114"/>
+      <c r="AN15" s="73"/>
+      <c r="AO15" s="76"/>
     </row>
     <row r="16" spans="1:41" s="15" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="91" t="s">
+      <c r="A16" s="88" t="s">
         <v>48</v>
       </c>
       <c r="B16" s="55"/>
@@ -3782,18 +3782,18 @@
       <c r="AD16" s="55"/>
       <c r="AE16" s="55"/>
       <c r="AF16" s="56"/>
-      <c r="AG16" s="93"/>
-      <c r="AH16" s="115"/>
-      <c r="AI16" s="102"/>
-      <c r="AJ16" s="102"/>
-      <c r="AK16" s="102"/>
-      <c r="AL16" s="101"/>
-      <c r="AM16" s="101"/>
-      <c r="AN16" s="102"/>
-      <c r="AO16" s="104"/>
+      <c r="AG16" s="90"/>
+      <c r="AH16" s="92"/>
+      <c r="AI16" s="82"/>
+      <c r="AJ16" s="82"/>
+      <c r="AK16" s="82"/>
+      <c r="AL16" s="84"/>
+      <c r="AM16" s="84"/>
+      <c r="AN16" s="82"/>
+      <c r="AO16" s="86"/>
     </row>
     <row r="17" spans="1:41" s="15" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="92"/>
+      <c r="A17" s="89"/>
       <c r="B17" s="22"/>
       <c r="C17" s="22"/>
       <c r="D17" s="22"/>
@@ -3825,15 +3825,15 @@
       <c r="AD17" s="22"/>
       <c r="AE17" s="22"/>
       <c r="AF17" s="23"/>
-      <c r="AG17" s="94"/>
-      <c r="AH17" s="116"/>
-      <c r="AI17" s="103"/>
-      <c r="AJ17" s="103"/>
-      <c r="AK17" s="103"/>
-      <c r="AL17" s="98"/>
-      <c r="AM17" s="98"/>
-      <c r="AN17" s="103"/>
-      <c r="AO17" s="105"/>
+      <c r="AG17" s="91"/>
+      <c r="AH17" s="93"/>
+      <c r="AI17" s="83"/>
+      <c r="AJ17" s="83"/>
+      <c r="AK17" s="83"/>
+      <c r="AL17" s="85"/>
+      <c r="AM17" s="85"/>
+      <c r="AN17" s="83"/>
+      <c r="AO17" s="87"/>
     </row>
     <row r="18" spans="1:41" s="17" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="16" t="s">
@@ -3870,15 +3870,15 @@
       <c r="AD18" s="24"/>
       <c r="AE18" s="24"/>
       <c r="AF18" s="25"/>
-      <c r="AG18" s="106"/>
-      <c r="AH18" s="108"/>
-      <c r="AI18" s="110"/>
-      <c r="AJ18" s="110"/>
-      <c r="AK18" s="110"/>
-      <c r="AL18" s="110"/>
+      <c r="AG18" s="78"/>
+      <c r="AH18" s="80"/>
+      <c r="AI18" s="72"/>
+      <c r="AJ18" s="72"/>
+      <c r="AK18" s="72"/>
+      <c r="AL18" s="72"/>
       <c r="AM18" s="63"/>
-      <c r="AN18" s="112"/>
-      <c r="AO18" s="113"/>
+      <c r="AN18" s="74"/>
+      <c r="AO18" s="75"/>
     </row>
     <row r="19" spans="1:41" s="17" customFormat="1" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="18" t="s">
@@ -3915,15 +3915,15 @@
       <c r="AD19" s="26"/>
       <c r="AE19" s="26"/>
       <c r="AF19" s="27"/>
-      <c r="AG19" s="107"/>
-      <c r="AH19" s="109"/>
-      <c r="AI19" s="111"/>
-      <c r="AJ19" s="111"/>
-      <c r="AK19" s="111"/>
-      <c r="AL19" s="111"/>
+      <c r="AG19" s="79"/>
+      <c r="AH19" s="81"/>
+      <c r="AI19" s="73"/>
+      <c r="AJ19" s="73"/>
+      <c r="AK19" s="73"/>
+      <c r="AL19" s="73"/>
       <c r="AM19" s="62"/>
-      <c r="AN19" s="111"/>
-      <c r="AO19" s="114"/>
+      <c r="AN19" s="73"/>
+      <c r="AO19" s="76"/>
     </row>
     <row r="20" spans="1:41" s="17" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="65"/>
@@ -4144,11 +4144,11 @@
       <c r="B25" s="64" t="s">
         <v>50</v>
       </c>
-      <c r="C25" s="117" t="s">
+      <c r="C25" s="70" t="s">
         <v>51</v>
       </c>
-      <c r="D25" s="117"/>
-      <c r="E25" s="117"/>
+      <c r="D25" s="70"/>
+      <c r="E25" s="70"/>
       <c r="F25" s="32"/>
       <c r="G25" s="32"/>
       <c r="H25" s="64" t="s">
@@ -4160,20 +4160,20 @@
       <c r="J25" s="32"/>
       <c r="K25" s="32"/>
       <c r="L25" s="32"/>
-      <c r="N25" s="119" t="s">
+      <c r="N25" s="77" t="s">
         <v>54</v>
       </c>
-      <c r="O25" s="119"/>
-      <c r="P25" s="119"/>
-      <c r="Q25" s="119"/>
-      <c r="R25" s="119"/>
-      <c r="T25" s="119" t="s">
+      <c r="O25" s="77"/>
+      <c r="P25" s="77"/>
+      <c r="Q25" s="77"/>
+      <c r="R25" s="77"/>
+      <c r="T25" s="77" t="s">
         <v>55</v>
       </c>
-      <c r="U25" s="119"/>
-      <c r="V25" s="119"/>
-      <c r="W25" s="119"/>
-      <c r="X25" s="119"/>
+      <c r="U25" s="77"/>
+      <c r="V25" s="77"/>
+      <c r="W25" s="77"/>
+      <c r="X25" s="77"/>
       <c r="Z25" s="33" t="s">
         <v>56</v>
       </c>
@@ -4185,64 +4185,64 @@
       <c r="AM25" s="19"/>
     </row>
     <row r="26" spans="1:41" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B26" s="117" t="s">
+      <c r="B26" s="70" t="s">
         <v>57</v>
       </c>
-      <c r="C26" s="117"/>
-      <c r="D26" s="117"/>
-      <c r="E26" s="117"/>
-      <c r="F26" s="117"/>
-      <c r="G26" s="117"/>
-      <c r="H26" s="117"/>
-      <c r="I26" s="117"/>
-      <c r="J26" s="117"/>
-      <c r="K26" s="117"/>
-      <c r="L26" s="117"/>
-      <c r="M26" s="117"/>
-      <c r="N26" s="117"/>
-      <c r="O26" s="117"/>
-      <c r="P26" s="117"/>
-      <c r="Q26" s="117"/>
-      <c r="R26" s="117"/>
-      <c r="S26" s="117"/>
-      <c r="T26" s="117"/>
-      <c r="U26" s="117"/>
-      <c r="V26" s="117"/>
-      <c r="W26" s="117"/>
-      <c r="X26" s="117"/>
-      <c r="Y26" s="117"/>
-      <c r="Z26" s="117"/>
-      <c r="AA26" s="117"/>
-      <c r="AB26" s="117"/>
-      <c r="AC26" s="117"/>
-      <c r="AD26" s="117"/>
-      <c r="AE26" s="117"/>
-      <c r="AF26" s="117"/>
-      <c r="AG26" s="117"/>
-      <c r="AH26" s="117"/>
-      <c r="AI26" s="117"/>
-      <c r="AJ26" s="117"/>
-      <c r="AK26" s="117"/>
-      <c r="AL26" s="117"/>
-      <c r="AM26" s="117"/>
-      <c r="AN26" s="117"/>
-      <c r="AO26" s="117"/>
+      <c r="C26" s="70"/>
+      <c r="D26" s="70"/>
+      <c r="E26" s="70"/>
+      <c r="F26" s="70"/>
+      <c r="G26" s="70"/>
+      <c r="H26" s="70"/>
+      <c r="I26" s="70"/>
+      <c r="J26" s="70"/>
+      <c r="K26" s="70"/>
+      <c r="L26" s="70"/>
+      <c r="M26" s="70"/>
+      <c r="N26" s="70"/>
+      <c r="O26" s="70"/>
+      <c r="P26" s="70"/>
+      <c r="Q26" s="70"/>
+      <c r="R26" s="70"/>
+      <c r="S26" s="70"/>
+      <c r="T26" s="70"/>
+      <c r="U26" s="70"/>
+      <c r="V26" s="70"/>
+      <c r="W26" s="70"/>
+      <c r="X26" s="70"/>
+      <c r="Y26" s="70"/>
+      <c r="Z26" s="70"/>
+      <c r="AA26" s="70"/>
+      <c r="AB26" s="70"/>
+      <c r="AC26" s="70"/>
+      <c r="AD26" s="70"/>
+      <c r="AE26" s="70"/>
+      <c r="AF26" s="70"/>
+      <c r="AG26" s="70"/>
+      <c r="AH26" s="70"/>
+      <c r="AI26" s="70"/>
+      <c r="AJ26" s="70"/>
+      <c r="AK26" s="70"/>
+      <c r="AL26" s="70"/>
+      <c r="AM26" s="70"/>
+      <c r="AN26" s="70"/>
+      <c r="AO26" s="70"/>
     </row>
     <row r="27" spans="1:41" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="34"/>
-      <c r="B27" s="118" t="s">
-        <v>71</v>
-      </c>
-      <c r="C27" s="118"/>
-      <c r="D27" s="118"/>
-      <c r="E27" s="118"/>
-      <c r="F27" s="118"/>
-      <c r="G27" s="118"/>
-      <c r="H27" s="118"/>
-      <c r="I27" s="118"/>
-      <c r="J27" s="118"/>
-      <c r="K27" s="118"/>
-      <c r="L27" s="118"/>
+      <c r="B27" s="71" t="s">
+        <v>70</v>
+      </c>
+      <c r="C27" s="71"/>
+      <c r="D27" s="71"/>
+      <c r="E27" s="71"/>
+      <c r="F27" s="71"/>
+      <c r="G27" s="71"/>
+      <c r="H27" s="71"/>
+      <c r="I27" s="71"/>
+      <c r="J27" s="71"/>
+      <c r="K27" s="71"/>
+      <c r="L27" s="71"/>
       <c r="M27" s="20"/>
       <c r="N27" s="20"/>
       <c r="O27" s="20"/>
@@ -4582,6 +4582,43 @@
     </row>
   </sheetData>
   <mergeCells count="50">
+    <mergeCell ref="A1:AO1"/>
+    <mergeCell ref="A2:AO2"/>
+    <mergeCell ref="A3:AO3"/>
+    <mergeCell ref="AG4:AG9"/>
+    <mergeCell ref="AH4:AL4"/>
+    <mergeCell ref="AO4:AO5"/>
+    <mergeCell ref="AH5:AN5"/>
+    <mergeCell ref="AH7:AL7"/>
+    <mergeCell ref="AH8:AN9"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="AG12:AG13"/>
+    <mergeCell ref="AH12:AH13"/>
+    <mergeCell ref="AI12:AI13"/>
+    <mergeCell ref="AJ12:AJ13"/>
+    <mergeCell ref="AL12:AL13"/>
+    <mergeCell ref="AM12:AM13"/>
+    <mergeCell ref="AN12:AN13"/>
+    <mergeCell ref="AO12:AO13"/>
+    <mergeCell ref="AG14:AG15"/>
+    <mergeCell ref="AH14:AH15"/>
+    <mergeCell ref="AI14:AI15"/>
+    <mergeCell ref="AJ14:AJ15"/>
+    <mergeCell ref="AK14:AK15"/>
+    <mergeCell ref="AL14:AL15"/>
+    <mergeCell ref="AK12:AK13"/>
+    <mergeCell ref="AN14:AN15"/>
+    <mergeCell ref="AO14:AO15"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="AG16:AG17"/>
+    <mergeCell ref="AH16:AH17"/>
+    <mergeCell ref="AI16:AI17"/>
+    <mergeCell ref="AJ16:AJ17"/>
+    <mergeCell ref="AK16:AK17"/>
+    <mergeCell ref="AL16:AL17"/>
+    <mergeCell ref="AM16:AM17"/>
+    <mergeCell ref="AN16:AN17"/>
+    <mergeCell ref="AO16:AO17"/>
     <mergeCell ref="B26:AO26"/>
     <mergeCell ref="B27:L27"/>
     <mergeCell ref="AL18:AL19"/>
@@ -4595,43 +4632,6 @@
     <mergeCell ref="AI18:AI19"/>
     <mergeCell ref="AJ18:AJ19"/>
     <mergeCell ref="AK18:AK19"/>
-    <mergeCell ref="AK16:AK17"/>
-    <mergeCell ref="AL16:AL17"/>
-    <mergeCell ref="AM16:AM17"/>
-    <mergeCell ref="AN16:AN17"/>
-    <mergeCell ref="AO16:AO17"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="AG16:AG17"/>
-    <mergeCell ref="AH16:AH17"/>
-    <mergeCell ref="AI16:AI17"/>
-    <mergeCell ref="AJ16:AJ17"/>
-    <mergeCell ref="AL12:AL13"/>
-    <mergeCell ref="AM12:AM13"/>
-    <mergeCell ref="AN12:AN13"/>
-    <mergeCell ref="AO12:AO13"/>
-    <mergeCell ref="AG14:AG15"/>
-    <mergeCell ref="AH14:AH15"/>
-    <mergeCell ref="AI14:AI15"/>
-    <mergeCell ref="AJ14:AJ15"/>
-    <mergeCell ref="AK14:AK15"/>
-    <mergeCell ref="AL14:AL15"/>
-    <mergeCell ref="AK12:AK13"/>
-    <mergeCell ref="AN14:AN15"/>
-    <mergeCell ref="AO14:AO15"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="AG12:AG13"/>
-    <mergeCell ref="AH12:AH13"/>
-    <mergeCell ref="AI12:AI13"/>
-    <mergeCell ref="AJ12:AJ13"/>
-    <mergeCell ref="A1:AO1"/>
-    <mergeCell ref="A2:AO2"/>
-    <mergeCell ref="A3:AO3"/>
-    <mergeCell ref="AG4:AG9"/>
-    <mergeCell ref="AH4:AL4"/>
-    <mergeCell ref="AO4:AO5"/>
-    <mergeCell ref="AH5:AN5"/>
-    <mergeCell ref="AH7:AL7"/>
-    <mergeCell ref="AH8:AN9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="75" fitToHeight="0" orientation="landscape" r:id="rId1"/>

</xml_diff>